<commit_message>
Time Fix and Exploratory Analysis_2
</commit_message>
<xml_diff>
--- a/data/raw_data/RAW_WQ Data_TimeModified.xlsx
+++ b/data/raw_data/RAW_WQ Data_TimeModified.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17033\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17033\Desktop\Modern Applied Data Analysis\William-Norfolk-Project\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917DE37C-9FE1-4A99-BEEB-2A38175C03F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9907DD-C97E-40B1-A18B-D1A64FC02060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3005" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3203" uniqueCount="756">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2120,6 +2120,174 @@
   </si>
   <si>
     <t>06.29.18</t>
+  </si>
+  <si>
+    <t>1605</t>
+  </si>
+  <si>
+    <t>1645</t>
+  </si>
+  <si>
+    <t>1230</t>
+  </si>
+  <si>
+    <t>1139</t>
+  </si>
+  <si>
+    <t>1157</t>
+  </si>
+  <si>
+    <t>1252</t>
+  </si>
+  <si>
+    <t>1508</t>
+  </si>
+  <si>
+    <t>1503</t>
+  </si>
+  <si>
+    <t>0947</t>
+  </si>
+  <si>
+    <t>1005</t>
+  </si>
+  <si>
+    <t>1426</t>
+  </si>
+  <si>
+    <t>1057</t>
+  </si>
+  <si>
+    <t>1054</t>
+  </si>
+  <si>
+    <t>1007</t>
+  </si>
+  <si>
+    <t>1521</t>
+  </si>
+  <si>
+    <t>1028</t>
+  </si>
+  <si>
+    <t>1440</t>
+  </si>
+  <si>
+    <t>1543</t>
+  </si>
+  <si>
+    <t>1627</t>
+  </si>
+  <si>
+    <t>1103</t>
+  </si>
+  <si>
+    <t>1447</t>
+  </si>
+  <si>
+    <t>1452</t>
+  </si>
+  <si>
+    <t>1118</t>
+  </si>
+  <si>
+    <t>1439</t>
+  </si>
+  <si>
+    <t>1632</t>
+  </si>
+  <si>
+    <t>1635</t>
+  </si>
+  <si>
+    <t>1409</t>
+  </si>
+  <si>
+    <t>1443</t>
+  </si>
+  <si>
+    <t>1548</t>
+  </si>
+  <si>
+    <t>1235</t>
+  </si>
+  <si>
+    <t>1319</t>
+  </si>
+  <si>
+    <t>0925</t>
+  </si>
+  <si>
+    <t>1444</t>
+  </si>
+  <si>
+    <t>1427</t>
+  </si>
+  <si>
+    <t>0943</t>
+  </si>
+  <si>
+    <t>1622</t>
+  </si>
+  <si>
+    <t>1046</t>
+  </si>
+  <si>
+    <t>1425</t>
+  </si>
+  <si>
+    <t>1539</t>
+  </si>
+  <si>
+    <t>1059</t>
+  </si>
+  <si>
+    <t>1009</t>
+  </si>
+  <si>
+    <t>0946</t>
+  </si>
+  <si>
+    <t>1436</t>
+  </si>
+  <si>
+    <t>1517</t>
+  </si>
+  <si>
+    <t>0936</t>
+  </si>
+  <si>
+    <t>1036</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1136</t>
+  </si>
+  <si>
+    <t>1016</t>
+  </si>
+  <si>
+    <t>0956</t>
+  </si>
+  <si>
+    <t>1538</t>
+  </si>
+  <si>
+    <t>1518</t>
+  </si>
+  <si>
+    <t>1644</t>
+  </si>
+  <si>
+    <t>1549</t>
+  </si>
+  <si>
+    <t>1531</t>
+  </si>
+  <si>
+    <t>1639</t>
   </si>
 </sst>
 </file>
@@ -2551,8 +2719,8 @@
   <dimension ref="A1:O902"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B302" sqref="B302"/>
+      <pane ySplit="1" topLeftCell="A500" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E524" sqref="E524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16129,7 +16297,9 @@
       <c r="D326" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E326" s="20"/>
+      <c r="E326" s="20" t="s">
+        <v>316</v>
+      </c>
       <c r="F326" s="1" t="s">
         <v>14</v>
       </c>
@@ -16168,7 +16338,9 @@
       <c r="D327" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E327" s="19"/>
+      <c r="E327" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F327" s="1" t="s">
         <v>71</v>
       </c>
@@ -16207,7 +16379,9 @@
       <c r="D328" s="7">
         <v>0.47222222222222221</v>
       </c>
-      <c r="E328" s="19"/>
+      <c r="E328" s="19" t="s">
+        <v>359</v>
+      </c>
       <c r="F328" s="1" t="s">
         <v>220</v>
       </c>
@@ -16246,7 +16420,9 @@
       <c r="D329" s="7">
         <v>0.63888888888888884</v>
       </c>
-      <c r="E329" s="19"/>
+      <c r="E329" s="19" t="s">
+        <v>328</v>
+      </c>
       <c r="F329" s="1" t="s">
         <v>5</v>
       </c>
@@ -16285,7 +16461,9 @@
       <c r="D330" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E330" s="19"/>
+      <c r="E330" s="19" t="s">
+        <v>363</v>
+      </c>
       <c r="F330" s="1" t="s">
         <v>10</v>
       </c>
@@ -16324,7 +16502,9 @@
       <c r="D331" s="7">
         <v>0.67013888888888884</v>
       </c>
-      <c r="E331" s="19"/>
+      <c r="E331" s="19" t="s">
+        <v>700</v>
+      </c>
       <c r="F331" s="1" t="s">
         <v>10</v>
       </c>
@@ -16363,7 +16543,9 @@
       <c r="D332" s="7">
         <v>0.69791666666666663</v>
       </c>
-      <c r="E332" s="19"/>
+      <c r="E332" s="19" t="s">
+        <v>701</v>
+      </c>
       <c r="F332" s="1" t="s">
         <v>12</v>
       </c>
@@ -16402,7 +16584,9 @@
       <c r="D333" s="7">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E333" s="19"/>
+      <c r="E333" s="19" t="s">
+        <v>421</v>
+      </c>
       <c r="F333" s="1" t="s">
         <v>87</v>
       </c>
@@ -16441,7 +16625,9 @@
       <c r="D334" s="7">
         <v>0.48541666666666666</v>
       </c>
-      <c r="E334" s="19"/>
+      <c r="E334" s="19" t="s">
+        <v>703</v>
+      </c>
       <c r="F334" s="1" t="s">
         <v>10</v>
       </c>
@@ -16480,7 +16666,9 @@
       <c r="D335" s="7">
         <v>0.5</v>
       </c>
-      <c r="E335" s="19"/>
+      <c r="E335" s="19" t="s">
+        <v>432</v>
+      </c>
       <c r="F335" s="1" t="s">
         <v>10</v>
       </c>
@@ -16519,7 +16707,9 @@
       <c r="D336" s="7">
         <v>0.49791666666666667</v>
       </c>
-      <c r="E336" s="19"/>
+      <c r="E336" s="19" t="s">
+        <v>704</v>
+      </c>
       <c r="F336" s="1" t="s">
         <v>10</v>
       </c>
@@ -16558,7 +16748,9 @@
       <c r="D337" s="7">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E337" s="19"/>
+      <c r="E337" s="19" t="s">
+        <v>389</v>
+      </c>
       <c r="F337" s="1" t="s">
         <v>133</v>
       </c>
@@ -16597,7 +16789,9 @@
       <c r="D338" s="7">
         <v>0.52083333333333337</v>
       </c>
-      <c r="E338" s="19"/>
+      <c r="E338" s="19" t="s">
+        <v>702</v>
+      </c>
       <c r="F338" s="1" t="s">
         <v>10</v>
       </c>
@@ -16636,7 +16830,9 @@
       <c r="D339" s="7">
         <v>0.53611111111111109</v>
       </c>
-      <c r="E339" s="19"/>
+      <c r="E339" s="19" t="s">
+        <v>705</v>
+      </c>
       <c r="F339" s="1" t="s">
         <v>21</v>
       </c>
@@ -16675,7 +16871,9 @@
       <c r="D340" s="7">
         <v>0.40902777777777777</v>
       </c>
-      <c r="E340" s="19"/>
+      <c r="E340" s="19" t="s">
+        <v>436</v>
+      </c>
       <c r="F340" s="1" t="s">
         <v>87</v>
       </c>
@@ -16714,7 +16912,9 @@
       <c r="D341" s="7">
         <v>0.4597222222222222</v>
       </c>
-      <c r="E341" s="19"/>
+      <c r="E341" s="19" t="s">
+        <v>384</v>
+      </c>
       <c r="F341" s="1" t="s">
         <v>175</v>
       </c>
@@ -16753,7 +16953,9 @@
       <c r="D342" s="7">
         <v>0.625</v>
       </c>
-      <c r="E342" s="19"/>
+      <c r="E342" s="19" t="s">
+        <v>346</v>
+      </c>
       <c r="F342" s="1" t="s">
         <v>10</v>
       </c>
@@ -16792,7 +16994,9 @@
       <c r="D343" s="7">
         <v>0.64861111111111114</v>
       </c>
-      <c r="E343" s="19"/>
+      <c r="E343" s="19" t="s">
+        <v>398</v>
+      </c>
       <c r="F343" s="1" t="s">
         <v>10</v>
       </c>
@@ -16831,7 +17035,9 @@
       <c r="D344" s="7">
         <v>0.64861111111111114</v>
       </c>
-      <c r="E344" s="19"/>
+      <c r="E344" s="19" t="s">
+        <v>398</v>
+      </c>
       <c r="F344" s="1" t="s">
         <v>15</v>
       </c>
@@ -16870,7 +17076,9 @@
       <c r="D345" s="7">
         <v>0.68055555555555558</v>
       </c>
-      <c r="E345" s="19"/>
+      <c r="E345" s="19" t="s">
+        <v>340</v>
+      </c>
       <c r="F345" s="1" t="s">
         <v>133</v>
       </c>
@@ -16909,7 +17117,9 @@
       <c r="D346" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E346" s="19"/>
+      <c r="E346" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F346" s="1" t="s">
         <v>10</v>
       </c>
@@ -16948,7 +17158,9 @@
       <c r="D347" s="7">
         <v>0.41319444444444442</v>
       </c>
-      <c r="E347" s="19"/>
+      <c r="E347" s="19" t="s">
+        <v>326</v>
+      </c>
       <c r="F347" s="1" t="s">
         <v>22</v>
       </c>
@@ -16987,7 +17199,9 @@
       <c r="D348" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E348" s="19"/>
+      <c r="E348" s="19" t="s">
+        <v>317</v>
+      </c>
       <c r="F348" s="1" t="s">
         <v>22</v>
       </c>
@@ -17026,7 +17240,9 @@
       <c r="D349" s="7">
         <v>0.63055555555555554</v>
       </c>
-      <c r="E349" s="19"/>
+      <c r="E349" s="19" t="s">
+        <v>706</v>
+      </c>
       <c r="F349" s="1" t="s">
         <v>87</v>
       </c>
@@ -17065,7 +17281,9 @@
       <c r="D350" s="7">
         <v>0.69791666666666663</v>
       </c>
-      <c r="E350" s="19"/>
+      <c r="E350" s="19" t="s">
+        <v>701</v>
+      </c>
       <c r="F350" s="1" t="s">
         <v>22</v>
       </c>
@@ -17104,7 +17322,9 @@
       <c r="D351" s="7">
         <v>0.62708333333333333</v>
       </c>
-      <c r="E351" s="19"/>
+      <c r="E351" s="19" t="s">
+        <v>707</v>
+      </c>
       <c r="F351" s="1" t="s">
         <v>9</v>
       </c>
@@ -17143,7 +17363,9 @@
       <c r="D352" s="7">
         <v>0.40763888888888888</v>
       </c>
-      <c r="E352" s="19"/>
+      <c r="E352" s="19" t="s">
+        <v>708</v>
+      </c>
       <c r="F352" s="1" t="s">
         <v>15</v>
       </c>
@@ -17182,7 +17404,9 @@
       <c r="D353" s="7">
         <v>0.40902777777777777</v>
       </c>
-      <c r="E353" s="19"/>
+      <c r="E353" s="19" t="s">
+        <v>436</v>
+      </c>
       <c r="F353" s="1" t="s">
         <v>133</v>
       </c>
@@ -17221,7 +17445,9 @@
       <c r="D354" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E354" s="19"/>
+      <c r="E354" s="19" t="s">
+        <v>356</v>
+      </c>
       <c r="F354" s="1" t="s">
         <v>10</v>
       </c>
@@ -17260,7 +17486,9 @@
       <c r="D355" s="7">
         <v>0.40972222222222221</v>
       </c>
-      <c r="E355" s="19"/>
+      <c r="E355" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="F355" s="1" t="s">
         <v>113</v>
       </c>
@@ -17299,7 +17527,9 @@
       <c r="D356" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E356" s="19"/>
+      <c r="E356" s="19" t="s">
+        <v>317</v>
+      </c>
       <c r="F356" s="1" t="s">
         <v>5</v>
       </c>
@@ -17338,7 +17568,9 @@
       <c r="D357" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E357" s="19"/>
+      <c r="E357" s="19" t="s">
+        <v>317</v>
+      </c>
       <c r="F357" s="1" t="s">
         <v>19</v>
       </c>
@@ -17377,7 +17609,9 @@
       <c r="D358" s="7">
         <v>0.40277777777777779</v>
       </c>
-      <c r="E358" s="19"/>
+      <c r="E358" s="19" t="s">
+        <v>434</v>
+      </c>
       <c r="F358" s="1" t="s">
         <v>10</v>
       </c>
@@ -17416,7 +17650,9 @@
       <c r="D359" s="7">
         <v>0.4201388888888889</v>
       </c>
-      <c r="E359" s="19"/>
+      <c r="E359" s="19" t="s">
+        <v>709</v>
+      </c>
       <c r="F359" s="1" t="s">
         <v>10</v>
       </c>
@@ -17455,7 +17691,9 @@
       <c r="D360" s="7">
         <v>0.61250000000000004</v>
       </c>
-      <c r="E360" s="19"/>
+      <c r="E360" s="19" t="s">
+        <v>424</v>
+      </c>
       <c r="F360" s="1" t="s">
         <v>71</v>
       </c>
@@ -17494,7 +17732,9 @@
       <c r="D361" s="7">
         <v>0.625</v>
       </c>
-      <c r="E361" s="19"/>
+      <c r="E361" s="19" t="s">
+        <v>346</v>
+      </c>
       <c r="F361" s="1" t="s">
         <v>10</v>
       </c>
@@ -17533,7 +17773,9 @@
       <c r="D362" s="7">
         <v>0.65277777777777779</v>
       </c>
-      <c r="E362" s="19"/>
+      <c r="E362" s="19" t="s">
+        <v>344</v>
+      </c>
       <c r="F362" s="1" t="s">
         <v>9</v>
       </c>
@@ -17572,7 +17814,9 @@
       <c r="D363" s="7">
         <v>0.65625</v>
       </c>
-      <c r="E363" s="19"/>
+      <c r="E363" s="19" t="s">
+        <v>342</v>
+      </c>
       <c r="F363" s="1" t="s">
         <v>16</v>
       </c>
@@ -17611,7 +17855,9 @@
       <c r="D364" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E364" s="19"/>
+      <c r="E364" s="19" t="s">
+        <v>363</v>
+      </c>
       <c r="F364" s="1" t="s">
         <v>11</v>
       </c>
@@ -17650,7 +17896,9 @@
       <c r="D365" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E365" s="19"/>
+      <c r="E365" s="19" t="s">
+        <v>299</v>
+      </c>
       <c r="F365" s="1" t="s">
         <v>11</v>
       </c>
@@ -17689,7 +17937,9 @@
       <c r="D366" s="7">
         <v>0.60138888888888886</v>
       </c>
-      <c r="E366" s="19"/>
+      <c r="E366" s="19" t="s">
+        <v>710</v>
+      </c>
       <c r="F366" s="1" t="s">
         <v>231</v>
       </c>
@@ -17728,7 +17978,9 @@
       <c r="D367" s="7">
         <v>0.45624999999999999</v>
       </c>
-      <c r="E367" s="19"/>
+      <c r="E367" s="19" t="s">
+        <v>711</v>
+      </c>
       <c r="F367" s="1" t="s">
         <v>14</v>
       </c>
@@ -17767,7 +18019,9 @@
       <c r="D368" s="7">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E368" s="19"/>
+      <c r="E368" s="19" t="s">
+        <v>350</v>
+      </c>
       <c r="F368" s="1" t="s">
         <v>11</v>
       </c>
@@ -17806,7 +18060,9 @@
       <c r="D369" s="7">
         <v>0.40763888888888888</v>
       </c>
-      <c r="E369" s="19"/>
+      <c r="E369" s="19" t="s">
+        <v>708</v>
+      </c>
       <c r="F369" s="1" t="s">
         <v>16</v>
       </c>
@@ -17845,7 +18101,9 @@
       <c r="D370" s="7">
         <v>0.45416666666666666</v>
       </c>
-      <c r="E370" s="19"/>
+      <c r="E370" s="19" t="s">
+        <v>712</v>
+      </c>
       <c r="F370" s="1" t="s">
         <v>22</v>
       </c>
@@ -17884,7 +18142,9 @@
       <c r="D371" s="7">
         <v>0.40902777777777777</v>
       </c>
-      <c r="E371" s="19"/>
+      <c r="E371" s="19" t="s">
+        <v>436</v>
+      </c>
       <c r="F371" s="1" t="s">
         <v>299</v>
       </c>
@@ -17923,7 +18183,9 @@
       <c r="D372" s="7">
         <v>0.42152777777777778</v>
       </c>
-      <c r="E372" s="19"/>
+      <c r="E372" s="19" t="s">
+        <v>713</v>
+      </c>
       <c r="F372" s="1" t="s">
         <v>10</v>
       </c>
@@ -17962,7 +18224,9 @@
       <c r="D373" s="7">
         <v>0.4465277777777778</v>
       </c>
-      <c r="E373" s="19"/>
+      <c r="E373" s="19" t="s">
+        <v>427</v>
+      </c>
       <c r="F373" s="1" t="s">
         <v>10</v>
       </c>
@@ -18001,7 +18265,9 @@
       <c r="D374" s="7">
         <v>0.46527777777777779</v>
       </c>
-      <c r="E374" s="19"/>
+      <c r="E374" s="19" t="s">
+        <v>416</v>
+      </c>
       <c r="F374" s="1" t="s">
         <v>19</v>
       </c>
@@ -18040,7 +18306,9 @@
       <c r="D375" s="7">
         <v>0.625</v>
       </c>
-      <c r="E375" s="19"/>
+      <c r="E375" s="19" t="s">
+        <v>346</v>
+      </c>
       <c r="F375" s="1" t="s">
         <v>11</v>
       </c>
@@ -18079,7 +18347,9 @@
       <c r="D376" s="7">
         <v>0.63888888888888884</v>
       </c>
-      <c r="E376" s="19"/>
+      <c r="E376" s="19" t="s">
+        <v>328</v>
+      </c>
       <c r="F376" s="1" t="s">
         <v>87</v>
       </c>
@@ -18118,7 +18388,9 @@
       <c r="D377" s="7">
         <v>0.63958333333333328</v>
       </c>
-      <c r="E377" s="19"/>
+      <c r="E377" s="19" t="s">
+        <v>714</v>
+      </c>
       <c r="F377" s="1" t="s">
         <v>16</v>
       </c>
@@ -18157,7 +18429,9 @@
       <c r="D378" s="7">
         <v>0.61458333333333337</v>
       </c>
-      <c r="E378" s="19"/>
+      <c r="E378" s="19" t="s">
+        <v>341</v>
+      </c>
       <c r="F378" s="1" t="s">
         <v>14</v>
       </c>
@@ -18196,7 +18470,9 @@
       <c r="D379" s="7">
         <v>0.39930555555555558</v>
       </c>
-      <c r="E379" s="19"/>
+      <c r="E379" s="19" t="s">
+        <v>380</v>
+      </c>
       <c r="F379" s="1" t="s">
         <v>15</v>
       </c>
@@ -18235,7 +18511,9 @@
       <c r="D380" s="7">
         <v>0.43402777777777779</v>
       </c>
-      <c r="E380" s="19"/>
+      <c r="E380" s="19" t="s">
+        <v>332</v>
+      </c>
       <c r="F380" s="1" t="s">
         <v>10</v>
       </c>
@@ -18274,7 +18552,9 @@
       <c r="D381" s="7">
         <v>0.43611111111111112</v>
       </c>
-      <c r="E381" s="19"/>
+      <c r="E381" s="19" t="s">
+        <v>715</v>
+      </c>
       <c r="F381" s="1" t="s">
         <v>10</v>
       </c>
@@ -18313,7 +18593,9 @@
       <c r="D382" s="7">
         <v>0.61111111111111116</v>
       </c>
-      <c r="E382" s="19"/>
+      <c r="E382" s="19" t="s">
+        <v>716</v>
+      </c>
       <c r="F382" s="1" t="s">
         <v>197</v>
       </c>
@@ -18352,7 +18634,9 @@
       <c r="D383" s="7">
         <v>0.61805555555555558</v>
       </c>
-      <c r="E383" s="19"/>
+      <c r="E383" s="19" t="s">
+        <v>361</v>
+      </c>
       <c r="F383" s="1" t="s">
         <v>10</v>
       </c>
@@ -18391,7 +18675,9 @@
       <c r="D384" s="7">
         <v>0.65625</v>
       </c>
-      <c r="E384" s="19"/>
+      <c r="E384" s="19" t="s">
+        <v>342</v>
+      </c>
       <c r="F384" s="1" t="s">
         <v>241</v>
       </c>
@@ -18430,7 +18716,9 @@
       <c r="D385" s="7">
         <v>0.62152777777777779</v>
       </c>
-      <c r="E385" s="19"/>
+      <c r="E385" s="19" t="s">
+        <v>413</v>
+      </c>
       <c r="F385" s="1" t="s">
         <v>197</v>
       </c>
@@ -18469,7 +18757,9 @@
       <c r="D386" s="7">
         <v>0.65486111111111112</v>
       </c>
-      <c r="E386" s="19"/>
+      <c r="E386" s="19" t="s">
+        <v>717</v>
+      </c>
       <c r="F386" s="1" t="s">
         <v>197</v>
       </c>
@@ -18508,7 +18798,9 @@
       <c r="D387" s="7">
         <v>0.65625</v>
       </c>
-      <c r="E387" s="19"/>
+      <c r="E387" s="19" t="s">
+        <v>342</v>
+      </c>
       <c r="F387" s="1" t="s">
         <v>197</v>
       </c>
@@ -18547,7 +18839,9 @@
       <c r="D388" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E388" s="19"/>
+      <c r="E388" s="19" t="s">
+        <v>316</v>
+      </c>
       <c r="F388" s="1" t="s">
         <v>11</v>
       </c>
@@ -18586,7 +18880,9 @@
       <c r="D389" s="7">
         <v>0.4826388888888889</v>
       </c>
-      <c r="E389" s="19"/>
+      <c r="E389" s="19" t="s">
+        <v>337</v>
+      </c>
       <c r="F389" s="1" t="s">
         <v>11</v>
       </c>
@@ -18625,7 +18921,9 @@
       <c r="D390" s="7">
         <v>0.63958333333333328</v>
       </c>
-      <c r="E390" s="19"/>
+      <c r="E390" s="19" t="s">
+        <v>714</v>
+      </c>
       <c r="F390" s="1" t="s">
         <v>11</v>
       </c>
@@ -18664,7 +18962,9 @@
       <c r="D391" s="7">
         <v>0.68541666666666667</v>
       </c>
-      <c r="E391" s="19"/>
+      <c r="E391" s="19" t="s">
+        <v>718</v>
+      </c>
       <c r="F391" s="1" t="s">
         <v>7</v>
       </c>
@@ -18703,7 +19003,9 @@
       <c r="D392" s="7">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E392" s="19"/>
+      <c r="E392" s="19" t="s">
+        <v>350</v>
+      </c>
       <c r="F392" s="1" t="s">
         <v>14</v>
       </c>
@@ -18742,7 +19044,9 @@
       <c r="D393" s="7">
         <v>0.40972222222222221</v>
       </c>
-      <c r="E393" s="19"/>
+      <c r="E393" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="F393" s="1" t="s">
         <v>14</v>
       </c>
@@ -18781,7 +19085,9 @@
       <c r="D394" s="7">
         <v>0.40972222222222221</v>
       </c>
-      <c r="E394" s="19"/>
+      <c r="E394" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="F394" s="1" t="s">
         <v>14</v>
       </c>
@@ -18820,7 +19126,9 @@
       <c r="D395" s="7">
         <v>0.46041666666666664</v>
       </c>
-      <c r="E395" s="19"/>
+      <c r="E395" s="19" t="s">
+        <v>719</v>
+      </c>
       <c r="F395" s="1" t="s">
         <v>245</v>
       </c>
@@ -18859,7 +19167,9 @@
       <c r="D396" s="7">
         <v>0.61597222222222225</v>
       </c>
-      <c r="E396" s="19"/>
+      <c r="E396" s="19" t="s">
+        <v>720</v>
+      </c>
       <c r="F396" s="1" t="s">
         <v>22</v>
       </c>
@@ -18898,7 +19208,9 @@
       <c r="D397" s="7">
         <v>0.61944444444444446</v>
       </c>
-      <c r="E397" s="19"/>
+      <c r="E397" s="19" t="s">
+        <v>721</v>
+      </c>
       <c r="F397" s="1" t="s">
         <v>22</v>
       </c>
@@ -18937,7 +19249,9 @@
       <c r="D398" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E398" s="19"/>
+      <c r="E398" s="19" t="s">
+        <v>317</v>
+      </c>
       <c r="F398" s="1" t="s">
         <v>7</v>
       </c>
@@ -18976,7 +19290,9 @@
       <c r="D399" s="7">
         <v>0.42083333333333334</v>
       </c>
-      <c r="E399" s="19"/>
+      <c r="E399" s="19" t="s">
+        <v>331</v>
+      </c>
       <c r="F399" s="1" t="s">
         <v>7</v>
       </c>
@@ -19015,7 +19331,9 @@
       <c r="D400" s="7">
         <v>0.4236111111111111</v>
       </c>
-      <c r="E400" s="19"/>
+      <c r="E400" s="19" t="s">
+        <v>429</v>
+      </c>
       <c r="F400" s="1" t="s">
         <v>16</v>
       </c>
@@ -19054,7 +19372,9 @@
       <c r="D401" s="7">
         <v>0.61458333333333337</v>
       </c>
-      <c r="E401" s="19"/>
+      <c r="E401" s="19" t="s">
+        <v>341</v>
+      </c>
       <c r="F401" s="1" t="s">
         <v>10</v>
       </c>
@@ -19093,7 +19413,9 @@
       <c r="D402" s="7">
         <v>0.46875</v>
       </c>
-      <c r="E402" s="19"/>
+      <c r="E402" s="19" t="s">
+        <v>352</v>
+      </c>
       <c r="F402" s="1" t="s">
         <v>248</v>
       </c>
@@ -19132,7 +19454,9 @@
       <c r="D403" s="7">
         <v>0.47083333333333333</v>
       </c>
-      <c r="E403" s="19"/>
+      <c r="E403" s="19" t="s">
+        <v>722</v>
+      </c>
       <c r="F403" s="1" t="s">
         <v>87</v>
       </c>
@@ -19171,7 +19495,9 @@
       <c r="D404" s="7">
         <v>0.61041666666666672</v>
       </c>
-      <c r="E404" s="19"/>
+      <c r="E404" s="19" t="s">
+        <v>723</v>
+      </c>
       <c r="F404" s="1" t="s">
         <v>10</v>
       </c>
@@ -19210,7 +19536,9 @@
       <c r="D405" s="7">
         <v>0.40972222222222221</v>
       </c>
-      <c r="E405" s="19"/>
+      <c r="E405" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="F405" s="1" t="s">
         <v>14</v>
       </c>
@@ -19249,7 +19577,9 @@
       <c r="D406" s="7">
         <v>0.40972222222222221</v>
       </c>
-      <c r="E406" s="19"/>
+      <c r="E406" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="F406" s="1" t="s">
         <v>14</v>
       </c>
@@ -19288,7 +19618,9 @@
       <c r="D407" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E407" s="19"/>
+      <c r="E407" s="19" t="s">
+        <v>316</v>
+      </c>
       <c r="F407" s="1" t="s">
         <v>71</v>
       </c>
@@ -19327,7 +19659,9 @@
       <c r="D408" s="7">
         <v>0.48194444444444445</v>
       </c>
-      <c r="E408" s="19"/>
+      <c r="E408" s="19" t="s">
+        <v>449</v>
+      </c>
       <c r="F408" s="1" t="s">
         <v>11</v>
       </c>
@@ -19366,7 +19700,9 @@
       <c r="D409" s="7">
         <v>0.65972222222222221</v>
       </c>
-      <c r="E409" s="19"/>
+      <c r="E409" s="19" t="s">
+        <v>357</v>
+      </c>
       <c r="F409" s="1" t="s">
         <v>71</v>
       </c>
@@ -19405,7 +19741,9 @@
       <c r="D410" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E410" s="19"/>
+      <c r="E410" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F410" s="1" t="s">
         <v>7</v>
       </c>
@@ -19444,7 +19782,9 @@
       <c r="D411" s="7">
         <v>0.625</v>
       </c>
-      <c r="E411" s="19"/>
+      <c r="E411" s="19" t="s">
+        <v>346</v>
+      </c>
       <c r="F411" s="1" t="s">
         <v>251</v>
       </c>
@@ -19483,7 +19823,9 @@
       <c r="D412" s="7">
         <v>0.64375000000000004</v>
       </c>
-      <c r="E412" s="19"/>
+      <c r="E412" s="19" t="s">
+        <v>414</v>
+      </c>
       <c r="F412" s="1" t="s">
         <v>15</v>
       </c>
@@ -19522,7 +19864,9 @@
       <c r="D413" s="7">
         <v>0.41319444444444442</v>
       </c>
-      <c r="E413" s="19"/>
+      <c r="E413" s="19" t="s">
+        <v>326</v>
+      </c>
       <c r="F413" s="1" t="s">
         <v>253</v>
       </c>
@@ -19561,7 +19905,9 @@
       <c r="D414" s="7">
         <v>0.4375</v>
       </c>
-      <c r="E414" s="19"/>
+      <c r="E414" s="19" t="s">
+        <v>311</v>
+      </c>
       <c r="F414" s="1" t="s">
         <v>87</v>
       </c>
@@ -19600,7 +19946,9 @@
       <c r="D415" s="7">
         <v>0.61597222222222225</v>
       </c>
-      <c r="E415" s="19"/>
+      <c r="E415" s="19" t="s">
+        <v>720</v>
+      </c>
       <c r="F415" s="1" t="s">
         <v>10</v>
       </c>
@@ -19639,7 +19987,9 @@
       <c r="D416" s="7">
         <v>0.39930555555555558</v>
       </c>
-      <c r="E416" s="19"/>
+      <c r="E416" s="19" t="s">
+        <v>380</v>
+      </c>
       <c r="F416" s="1" t="s">
         <v>14</v>
       </c>
@@ -19678,7 +20028,9 @@
       <c r="D417" s="7">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E417" s="19"/>
+      <c r="E417" s="19" t="s">
+        <v>408</v>
+      </c>
       <c r="F417" s="1" t="s">
         <v>120</v>
       </c>
@@ -19717,7 +20069,9 @@
       <c r="D418" s="7">
         <v>0.65625</v>
       </c>
-      <c r="E418" s="19"/>
+      <c r="E418" s="19" t="s">
+        <v>342</v>
+      </c>
       <c r="F418" s="1" t="s">
         <v>11</v>
       </c>
@@ -19756,7 +20110,9 @@
       <c r="D419" s="7">
         <v>0.68888888888888888</v>
       </c>
-      <c r="E419" s="19"/>
+      <c r="E419" s="19" t="s">
+        <v>724</v>
+      </c>
       <c r="F419" s="1" t="s">
         <v>7</v>
       </c>
@@ -19795,7 +20151,9 @@
       <c r="D420" s="7">
         <v>0.69097222222222221</v>
       </c>
-      <c r="E420" s="19"/>
+      <c r="E420" s="19" t="s">
+        <v>725</v>
+      </c>
       <c r="F420" s="1" t="s">
         <v>21</v>
       </c>
@@ -19834,7 +20192,9 @@
       <c r="D421" s="7">
         <v>0.40972222222222221</v>
       </c>
-      <c r="E421" s="19"/>
+      <c r="E421" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="F421" s="1" t="s">
         <v>21</v>
       </c>
@@ -19873,7 +20233,9 @@
       <c r="D422" s="7">
         <v>0.4201388888888889</v>
       </c>
-      <c r="E422" s="19"/>
+      <c r="E422" s="19" t="s">
+        <v>709</v>
+      </c>
       <c r="F422" s="1" t="s">
         <v>10</v>
       </c>
@@ -19912,7 +20274,9 @@
       <c r="D423" s="7">
         <v>0.46180555555555558</v>
       </c>
-      <c r="E423" s="19"/>
+      <c r="E423" s="19" t="s">
+        <v>445</v>
+      </c>
       <c r="F423" s="1" t="s">
         <v>120</v>
       </c>
@@ -19951,7 +20315,9 @@
       <c r="D424" s="7">
         <v>0.58958333333333335</v>
       </c>
-      <c r="E424" s="19"/>
+      <c r="E424" s="19" t="s">
+        <v>726</v>
+      </c>
       <c r="F424" s="1" t="s">
         <v>12</v>
       </c>
@@ -19990,7 +20356,9 @@
       <c r="D425" s="7">
         <v>0.61111111111111116</v>
       </c>
-      <c r="E425" s="19"/>
+      <c r="E425" s="19" t="s">
+        <v>716</v>
+      </c>
       <c r="F425" s="1" t="s">
         <v>107</v>
       </c>
@@ -20029,7 +20397,9 @@
       <c r="D426" s="7">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E426" s="19"/>
+      <c r="E426" s="19" t="s">
+        <v>323</v>
+      </c>
       <c r="F426" s="1" t="s">
         <v>9</v>
       </c>
@@ -20068,7 +20438,9 @@
       <c r="D427" s="7">
         <v>0.61319444444444449</v>
       </c>
-      <c r="E427" s="19"/>
+      <c r="E427" s="19" t="s">
+        <v>727</v>
+      </c>
       <c r="F427" s="1" t="s">
         <v>15</v>
       </c>
@@ -20107,7 +20479,9 @@
       <c r="D428" s="7">
         <v>0.63124999999999998</v>
       </c>
-      <c r="E428" s="19"/>
+      <c r="E428" s="19" t="s">
+        <v>446</v>
+      </c>
       <c r="F428" s="1" t="s">
         <v>14</v>
       </c>
@@ -20146,7 +20520,9 @@
       <c r="D429" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E429" s="19"/>
+      <c r="E429" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F429" s="1" t="s">
         <v>14</v>
       </c>
@@ -20185,7 +20561,9 @@
       <c r="D430" s="7">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E430" s="19"/>
+      <c r="E430" s="19" t="s">
+        <v>327</v>
+      </c>
       <c r="F430" s="1" t="s">
         <v>71</v>
       </c>
@@ -20224,7 +20602,9 @@
       <c r="D431" s="7">
         <v>0.47222222222222221</v>
       </c>
-      <c r="E431" s="19"/>
+      <c r="E431" s="19" t="s">
+        <v>359</v>
+      </c>
       <c r="F431" s="1" t="s">
         <v>15</v>
       </c>
@@ -20263,7 +20643,9 @@
       <c r="D432" s="7">
         <v>0.64444444444444449</v>
       </c>
-      <c r="E432" s="19"/>
+      <c r="E432" s="19" t="s">
+        <v>441</v>
+      </c>
       <c r="F432" s="1" t="s">
         <v>261</v>
       </c>
@@ -20302,7 +20684,9 @@
       <c r="D433" s="7">
         <v>0.65833333333333333</v>
       </c>
-      <c r="E433" s="19"/>
+      <c r="E433" s="19" t="s">
+        <v>728</v>
+      </c>
       <c r="F433" s="1" t="s">
         <v>261</v>
       </c>
@@ -20341,7 +20725,9 @@
       <c r="D434" s="7">
         <v>0.4201388888888889</v>
       </c>
-      <c r="E434" s="19"/>
+      <c r="E434" s="19" t="s">
+        <v>709</v>
+      </c>
       <c r="F434" s="1" t="s">
         <v>120</v>
       </c>
@@ -20380,7 +20766,9 @@
       <c r="D435" s="7">
         <v>0.5</v>
       </c>
-      <c r="E435" s="19"/>
+      <c r="E435" s="19" t="s">
+        <v>432</v>
+      </c>
       <c r="F435" s="1" t="s">
         <v>16</v>
       </c>
@@ -20419,7 +20807,9 @@
       <c r="D436" s="7">
         <v>0.52430555555555558</v>
       </c>
-      <c r="E436" s="19"/>
+      <c r="E436" s="19" t="s">
+        <v>729</v>
+      </c>
       <c r="F436" s="1" t="s">
         <v>11</v>
       </c>
@@ -20458,7 +20848,9 @@
       <c r="D437" s="7">
         <v>0.55486111111111114</v>
       </c>
-      <c r="E437" s="19"/>
+      <c r="E437" s="19" t="s">
+        <v>730</v>
+      </c>
       <c r="F437" s="1" t="s">
         <v>12</v>
       </c>
@@ -20497,7 +20889,9 @@
       <c r="D438" s="7">
         <v>0.3923611111111111</v>
       </c>
-      <c r="E438" s="19"/>
+      <c r="E438" s="19" t="s">
+        <v>731</v>
+      </c>
       <c r="F438" s="1" t="s">
         <v>12</v>
       </c>
@@ -20536,7 +20930,9 @@
       <c r="D439" s="7">
         <v>0.46736111111111112</v>
       </c>
-      <c r="E439" s="19"/>
+      <c r="E439" s="19" t="s">
+        <v>330</v>
+      </c>
       <c r="F439" s="1" t="s">
         <v>9</v>
       </c>
@@ -20575,7 +20971,9 @@
       <c r="D440" s="7">
         <v>0.68472222222222223</v>
       </c>
-      <c r="E440" s="19"/>
+      <c r="E440" s="19" t="s">
+        <v>397</v>
+      </c>
       <c r="F440" s="1" t="s">
         <v>22</v>
       </c>
@@ -20614,7 +21012,9 @@
       <c r="D441" s="7">
         <v>0.61388888888888893</v>
       </c>
-      <c r="E441" s="19"/>
+      <c r="E441" s="19" t="s">
+        <v>732</v>
+      </c>
       <c r="F441" s="1" t="s">
         <v>268</v>
       </c>
@@ -20653,7 +21053,9 @@
       <c r="D442" s="7">
         <v>0.65972222222222221</v>
       </c>
-      <c r="E442" s="19"/>
+      <c r="E442" s="19" t="s">
+        <v>357</v>
+      </c>
       <c r="F442" s="1" t="s">
         <v>10</v>
       </c>
@@ -20692,7 +21094,9 @@
       <c r="D443" s="7">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E443" s="19"/>
+      <c r="E443" s="19" t="s">
+        <v>323</v>
+      </c>
       <c r="F443" s="1" t="s">
         <v>11</v>
       </c>
@@ -20731,7 +21135,9 @@
       <c r="D444" s="7">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E444" s="19"/>
+      <c r="E444" s="19" t="s">
+        <v>350</v>
+      </c>
       <c r="F444" s="1" t="s">
         <v>13</v>
       </c>
@@ -20770,7 +21176,9 @@
       <c r="D445" s="7">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E445" s="19"/>
+      <c r="E445" s="19" t="s">
+        <v>323</v>
+      </c>
       <c r="F445" s="1" t="s">
         <v>19</v>
       </c>
@@ -20809,7 +21217,9 @@
       <c r="D446" s="7">
         <v>0.6020833333333333</v>
       </c>
-      <c r="E446" s="19"/>
+      <c r="E446" s="19" t="s">
+        <v>733</v>
+      </c>
       <c r="F446" s="1" t="s">
         <v>11</v>
       </c>
@@ -20848,7 +21258,9 @@
       <c r="D447" s="7">
         <v>0.4375</v>
       </c>
-      <c r="E447" s="19"/>
+      <c r="E447" s="19" t="s">
+        <v>311</v>
+      </c>
       <c r="F447" s="1" t="s">
         <v>16</v>
       </c>
@@ -20887,7 +21299,9 @@
       <c r="D448" s="7">
         <v>0.4375</v>
       </c>
-      <c r="E448" s="19"/>
+      <c r="E448" s="19" t="s">
+        <v>311</v>
+      </c>
       <c r="F448" s="1" t="s">
         <v>241</v>
       </c>
@@ -20926,7 +21340,9 @@
       <c r="D449" s="7">
         <v>0.63888888888888884</v>
       </c>
-      <c r="E449" s="19"/>
+      <c r="E449" s="19" t="s">
+        <v>328</v>
+      </c>
       <c r="F449" s="1" t="s">
         <v>87</v>
       </c>
@@ -20965,7 +21381,9 @@
       <c r="D450" s="7">
         <v>0.40486111111111112</v>
       </c>
-      <c r="E450" s="19"/>
+      <c r="E450" s="19" t="s">
+        <v>734</v>
+      </c>
       <c r="F450" s="1" t="s">
         <v>10</v>
       </c>
@@ -21004,7 +21422,9 @@
       <c r="D451" s="7">
         <v>0.64027777777777772</v>
       </c>
-      <c r="E451" s="19"/>
+      <c r="E451" s="19" t="s">
+        <v>409</v>
+      </c>
       <c r="F451" s="1" t="s">
         <v>20</v>
       </c>
@@ -21043,7 +21463,9 @@
       <c r="D452" s="7">
         <v>0.68194444444444446</v>
       </c>
-      <c r="E452" s="19"/>
+      <c r="E452" s="19" t="s">
+        <v>735</v>
+      </c>
       <c r="F452" s="1" t="s">
         <v>21</v>
       </c>
@@ -21082,7 +21504,9 @@
       <c r="D453" s="7">
         <v>0.40625</v>
       </c>
-      <c r="E453" s="19"/>
+      <c r="E453" s="19" t="s">
+        <v>345</v>
+      </c>
       <c r="F453" s="1" t="s">
         <v>14</v>
       </c>
@@ -21121,7 +21545,9 @@
       <c r="D454" s="7">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E454" s="19"/>
+      <c r="E454" s="19" t="s">
+        <v>327</v>
+      </c>
       <c r="F454" s="1" t="s">
         <v>120</v>
       </c>
@@ -21160,7 +21586,9 @@
       <c r="D455" s="7">
         <v>0.44861111111111113</v>
       </c>
-      <c r="E455" s="19"/>
+      <c r="E455" s="19" t="s">
+        <v>736</v>
+      </c>
       <c r="F455" s="1" t="s">
         <v>120</v>
       </c>
@@ -21199,7 +21627,9 @@
       <c r="D456" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E456" s="19"/>
+      <c r="E456" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F456" s="1" t="s">
         <v>10</v>
       </c>
@@ -21238,7 +21668,9 @@
       <c r="D457" s="7">
         <v>0.61458333333333337</v>
       </c>
-      <c r="E457" s="19"/>
+      <c r="E457" s="19" t="s">
+        <v>737</v>
+      </c>
       <c r="F457" s="1" t="s">
         <v>14</v>
       </c>
@@ -21277,7 +21709,9 @@
       <c r="D458" s="7">
         <v>0.66597222222222219</v>
       </c>
-      <c r="E458" s="19"/>
+      <c r="E458" s="19" t="s">
+        <v>738</v>
+      </c>
       <c r="F458" s="1" t="s">
         <v>14</v>
       </c>
@@ -21316,7 +21750,9 @@
       <c r="D459" s="7">
         <v>0.61458333333333337</v>
       </c>
-      <c r="E459" s="19"/>
+      <c r="E459" s="19" t="s">
+        <v>341</v>
+      </c>
       <c r="F459" s="1" t="s">
         <v>10</v>
       </c>
@@ -21355,7 +21791,9 @@
       <c r="D460" s="7">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E460" s="19"/>
+      <c r="E460" s="19" t="s">
+        <v>739</v>
+      </c>
       <c r="F460" s="1" t="s">
         <v>14</v>
       </c>
@@ -21394,7 +21832,9 @@
       <c r="D461" s="7">
         <v>0.65208333333333335</v>
       </c>
-      <c r="E461" s="19"/>
+      <c r="E461" s="19" t="s">
+        <v>738</v>
+      </c>
       <c r="F461" s="1" t="s">
         <v>87</v>
       </c>
@@ -21433,7 +21873,9 @@
       <c r="D462" s="7">
         <v>0.65277777777777779</v>
       </c>
-      <c r="E462" s="19"/>
+      <c r="E462" s="19" t="s">
+        <v>344</v>
+      </c>
       <c r="F462" s="1" t="s">
         <v>107</v>
       </c>
@@ -21472,7 +21914,9 @@
       <c r="D463" s="7">
         <v>0.42291666666666666</v>
       </c>
-      <c r="E463" s="19"/>
+      <c r="E463" s="19" t="s">
+        <v>740</v>
+      </c>
       <c r="F463" s="1" t="s">
         <v>9</v>
       </c>
@@ -21511,7 +21955,9 @@
       <c r="D464" s="7">
         <v>0.40694444444444444</v>
       </c>
-      <c r="E464" s="19"/>
+      <c r="E464" s="19" t="s">
+        <v>741</v>
+      </c>
       <c r="F464" s="1" t="s">
         <v>17</v>
       </c>
@@ -21550,7 +21996,9 @@
       <c r="D465" s="7">
         <v>0.40972222222222221</v>
       </c>
-      <c r="E465" s="19"/>
+      <c r="E465" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="F465" s="1" t="s">
         <v>11</v>
       </c>
@@ -21589,7 +22037,9 @@
       <c r="D466" s="7">
         <v>0.42291666666666666</v>
       </c>
-      <c r="E466" s="19"/>
+      <c r="E466" s="19" t="s">
+        <v>740</v>
+      </c>
       <c r="F466" s="1" t="s">
         <v>9</v>
       </c>
@@ -21628,7 +22078,9 @@
       <c r="D467" s="7">
         <v>0.4236111111111111</v>
       </c>
-      <c r="E467" s="19"/>
+      <c r="E467" s="19" t="s">
+        <v>429</v>
+      </c>
       <c r="F467" s="1" t="s">
         <v>7</v>
       </c>
@@ -21667,7 +22119,9 @@
       <c r="D468" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E468" s="19"/>
+      <c r="E468" s="19" t="s">
+        <v>316</v>
+      </c>
       <c r="F468" s="1" t="s">
         <v>16</v>
       </c>
@@ -21706,7 +22160,9 @@
       <c r="D469" s="7">
         <v>0.6118055555555556</v>
       </c>
-      <c r="E469" s="19"/>
+      <c r="E469" s="19" t="s">
+        <v>406</v>
+      </c>
       <c r="F469" s="1" t="s">
         <v>9</v>
       </c>
@@ -21745,7 +22201,9 @@
       <c r="D470" s="7">
         <v>0.60833333333333328</v>
       </c>
-      <c r="E470" s="19"/>
+      <c r="E470" s="19" t="s">
+        <v>742</v>
+      </c>
       <c r="F470" s="1" t="s">
         <v>13</v>
       </c>
@@ -21784,7 +22242,9 @@
       <c r="D471" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E471" s="19"/>
+      <c r="E471" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F471" s="1" t="s">
         <v>7</v>
       </c>
@@ -21823,7 +22283,9 @@
       <c r="D472" s="7">
         <v>0.3923611111111111</v>
       </c>
-      <c r="E472" s="19"/>
+      <c r="E472" s="19" t="s">
+        <v>731</v>
+      </c>
       <c r="F472" s="1" t="s">
         <v>19</v>
       </c>
@@ -21862,7 +22324,9 @@
       <c r="D473" s="7">
         <v>0.43263888888888891</v>
       </c>
-      <c r="E473" s="19"/>
+      <c r="E473" s="19" t="s">
+        <v>411</v>
+      </c>
       <c r="F473" s="1" t="s">
         <v>14</v>
       </c>
@@ -21901,7 +22365,9 @@
       <c r="D474" s="7">
         <v>0.43819444444444444</v>
       </c>
-      <c r="E474" s="19"/>
+      <c r="E474" s="19" t="s">
+        <v>443</v>
+      </c>
       <c r="F474" s="1" t="s">
         <v>14</v>
       </c>
@@ -21940,7 +22406,9 @@
       <c r="D475" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E475" s="19"/>
+      <c r="E475" s="19" t="s">
+        <v>356</v>
+      </c>
       <c r="F475" s="1" t="s">
         <v>278</v>
       </c>
@@ -21979,7 +22447,9 @@
       <c r="D476" s="7">
         <v>0.63680555555555551</v>
       </c>
-      <c r="E476" s="19"/>
+      <c r="E476" s="19" t="s">
+        <v>743</v>
+      </c>
       <c r="F476" s="1" t="s">
         <v>87</v>
       </c>
@@ -22018,7 +22488,9 @@
       <c r="D477" s="7">
         <v>0.64444444444444449</v>
       </c>
-      <c r="E477" s="19"/>
+      <c r="E477" s="19" t="s">
+        <v>441</v>
+      </c>
       <c r="F477" s="1" t="s">
         <v>13</v>
       </c>
@@ -22057,7 +22529,9 @@
       <c r="D478" s="7">
         <v>0.4</v>
       </c>
-      <c r="E478" s="19"/>
+      <c r="E478" s="19" t="s">
+        <v>744</v>
+      </c>
       <c r="F478" s="1" t="s">
         <v>280</v>
       </c>
@@ -22096,7 +22570,9 @@
       <c r="D479" s="7">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E479" s="19"/>
+      <c r="E479" s="19" t="s">
+        <v>422</v>
+      </c>
       <c r="F479" s="1" t="s">
         <v>20</v>
       </c>
@@ -22135,7 +22611,9 @@
       <c r="D480" s="7">
         <v>0.40625</v>
       </c>
-      <c r="E480" s="19"/>
+      <c r="E480" s="19" t="s">
+        <v>345</v>
+      </c>
       <c r="F480" s="1" t="s">
         <v>197</v>
       </c>
@@ -22174,7 +22652,9 @@
       <c r="D481" s="7">
         <v>0.40625</v>
       </c>
-      <c r="E481" s="19"/>
+      <c r="E481" s="19" t="s">
+        <v>345</v>
+      </c>
       <c r="F481" s="1" t="s">
         <v>13</v>
       </c>
@@ -22213,7 +22693,9 @@
       <c r="D482" s="7">
         <v>0.44166666666666665</v>
       </c>
-      <c r="E482" s="19"/>
+      <c r="E482" s="19" t="s">
+        <v>745</v>
+      </c>
       <c r="F482" s="1" t="s">
         <v>17</v>
       </c>
@@ -22252,7 +22734,9 @@
       <c r="D483" s="7">
         <v>0.44444444444444442</v>
       </c>
-      <c r="E483" s="19"/>
+      <c r="E483" s="19" t="s">
+        <v>362</v>
+      </c>
       <c r="F483" s="1" t="s">
         <v>87</v>
       </c>
@@ -22291,7 +22775,9 @@
       <c r="D484" s="7">
         <v>0.68194444444444446</v>
       </c>
-      <c r="E484" s="19"/>
+      <c r="E484" s="19" t="s">
+        <v>735</v>
+      </c>
       <c r="F484" s="1" t="s">
         <v>18</v>
       </c>
@@ -22330,7 +22816,9 @@
       <c r="D485" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E485" s="19"/>
+      <c r="E485" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F485" s="1" t="s">
         <v>18</v>
       </c>
@@ -22369,7 +22857,9 @@
       <c r="D486" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E486" s="19"/>
+      <c r="E486" s="19" t="s">
+        <v>299</v>
+      </c>
       <c r="F486" s="1" t="s">
         <v>87</v>
       </c>
@@ -22408,7 +22898,9 @@
       <c r="D487" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E487" s="19"/>
+      <c r="E487" s="19" t="s">
+        <v>317</v>
+      </c>
       <c r="F487" s="1" t="s">
         <v>14</v>
       </c>
@@ -22447,7 +22939,9 @@
       <c r="D488" s="7">
         <v>0.42430555555555555</v>
       </c>
-      <c r="E488" s="19"/>
+      <c r="E488" s="19" t="s">
+        <v>746</v>
+      </c>
       <c r="F488" s="1" t="s">
         <v>284</v>
       </c>
@@ -22486,7 +22980,9 @@
       <c r="D489" s="7">
         <v>0.48333333333333334</v>
       </c>
-      <c r="E489" s="19"/>
+      <c r="E489" s="19" t="s">
+        <v>747</v>
+      </c>
       <c r="F489" s="1" t="s">
         <v>120</v>
       </c>
@@ -22525,7 +23021,9 @@
       <c r="D490" s="7">
         <v>0.625</v>
       </c>
-      <c r="E490" s="19"/>
+      <c r="E490" s="19" t="s">
+        <v>346</v>
+      </c>
       <c r="F490" s="1" t="s">
         <v>57</v>
       </c>
@@ -22564,7 +23062,9 @@
       <c r="D491" s="7">
         <v>0.40833333333333333</v>
       </c>
-      <c r="E491" s="19"/>
+      <c r="E491" s="19" t="s">
+        <v>428</v>
+      </c>
       <c r="F491" s="1" t="s">
         <v>15</v>
       </c>
@@ -22603,7 +23103,9 @@
       <c r="D492" s="7">
         <v>0.42777777777777776</v>
       </c>
-      <c r="E492" s="19"/>
+      <c r="E492" s="19" t="s">
+        <v>748</v>
+      </c>
       <c r="F492" s="1" t="s">
         <v>15</v>
       </c>
@@ -22642,7 +23144,9 @@
       <c r="D493" s="7">
         <v>0.13541666666666666</v>
       </c>
-      <c r="E493" s="19"/>
+      <c r="E493" s="19" t="s">
+        <v>348</v>
+      </c>
       <c r="F493" s="1" t="s">
         <v>16</v>
       </c>
@@ -22681,7 +23185,9 @@
       <c r="D494" s="7">
         <v>0.65625</v>
       </c>
-      <c r="E494" s="19"/>
+      <c r="E494" s="19" t="s">
+        <v>342</v>
+      </c>
       <c r="F494" s="1" t="s">
         <v>18</v>
       </c>
@@ -22720,7 +23226,9 @@
       <c r="D495" s="7">
         <v>0.68402777777777779</v>
       </c>
-      <c r="E495" s="19"/>
+      <c r="E495" s="19" t="s">
+        <v>354</v>
+      </c>
       <c r="F495" s="1" t="s">
         <v>16</v>
       </c>
@@ -22759,7 +23267,9 @@
       <c r="D496" s="7">
         <v>0.43958333333333333</v>
       </c>
-      <c r="E496" s="19"/>
+      <c r="E496" s="19" t="s">
+        <v>435</v>
+      </c>
       <c r="F496" s="1" t="s">
         <v>10</v>
       </c>
@@ -22798,7 +23308,9 @@
       <c r="D497" s="7">
         <v>0.44097222222222221</v>
       </c>
-      <c r="E497" s="19"/>
+      <c r="E497" s="19" t="s">
+        <v>379</v>
+      </c>
       <c r="F497" s="1" t="s">
         <v>10</v>
       </c>
@@ -22837,7 +23349,9 @@
       <c r="D498" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E498" s="19"/>
+      <c r="E498" s="19" t="s">
+        <v>356</v>
+      </c>
       <c r="F498" s="1" t="s">
         <v>15</v>
       </c>
@@ -22876,7 +23390,9 @@
       <c r="D499" s="7">
         <v>0.41388888888888886</v>
       </c>
-      <c r="E499" s="19"/>
+      <c r="E499" s="19" t="s">
+        <v>749</v>
+      </c>
       <c r="F499" s="1" t="s">
         <v>14</v>
       </c>
@@ -22915,7 +23431,9 @@
       <c r="D500" s="7">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E500" s="19"/>
+      <c r="E500" s="19" t="s">
+        <v>323</v>
+      </c>
       <c r="F500" s="1" t="s">
         <v>241</v>
       </c>
@@ -22954,7 +23472,9 @@
       <c r="D501" s="7">
         <v>0.65138888888888891</v>
       </c>
-      <c r="E501" s="19"/>
+      <c r="E501" s="19" t="s">
+        <v>750</v>
+      </c>
       <c r="F501" s="1" t="s">
         <v>87</v>
       </c>
@@ -22993,7 +23513,9 @@
       <c r="D502" s="7">
         <v>0.69722222222222219</v>
       </c>
-      <c r="E502" s="19"/>
+      <c r="E502" s="19" t="s">
+        <v>752</v>
+      </c>
       <c r="F502" s="1" t="s">
         <v>11</v>
       </c>
@@ -23032,7 +23554,9 @@
       <c r="D503" s="7">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E503" s="19"/>
+      <c r="E503" s="19" t="s">
+        <v>323</v>
+      </c>
       <c r="F503" s="1" t="s">
         <v>87</v>
       </c>
@@ -23071,7 +23595,9 @@
       <c r="D504" s="7">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E504" s="19"/>
+      <c r="E504" s="19" t="s">
+        <v>348</v>
+      </c>
       <c r="F504" s="1" t="s">
         <v>288</v>
       </c>
@@ -23110,7 +23636,9 @@
       <c r="D505" s="7">
         <v>0.63888888888888884</v>
       </c>
-      <c r="E505" s="19"/>
+      <c r="E505" s="19" t="s">
+        <v>328</v>
+      </c>
       <c r="F505" s="1" t="s">
         <v>288</v>
       </c>
@@ -23149,7 +23677,9 @@
       <c r="D506" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E506" s="19"/>
+      <c r="E506" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F506" s="1" t="s">
         <v>288</v>
       </c>
@@ -23188,7 +23718,9 @@
       <c r="D507" s="7">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E507" s="19"/>
+      <c r="E507" s="19" t="s">
+        <v>323</v>
+      </c>
       <c r="F507" s="1" t="s">
         <v>10</v>
       </c>
@@ -23227,7 +23759,9 @@
       <c r="D508" s="7">
         <v>0.68055555555555558</v>
       </c>
-      <c r="E508" s="19"/>
+      <c r="E508" s="19" t="s">
+        <v>340</v>
+      </c>
       <c r="F508" s="1" t="s">
         <v>5</v>
       </c>
@@ -23266,7 +23800,9 @@
       <c r="D509" s="7">
         <v>0.6875</v>
       </c>
-      <c r="E509" s="19"/>
+      <c r="E509" s="19" t="s">
+        <v>373</v>
+      </c>
       <c r="F509" s="1" t="s">
         <v>5</v>
       </c>
@@ -23305,7 +23841,9 @@
       <c r="D510" s="10">
         <v>0.44583333333333336</v>
       </c>
-      <c r="E510" s="19"/>
+      <c r="E510" s="19" t="s">
+        <v>440</v>
+      </c>
       <c r="F510" s="1" t="s">
         <v>289</v>
       </c>
@@ -23344,7 +23882,9 @@
       <c r="D511" s="7">
         <v>0.46736111111111112</v>
       </c>
-      <c r="E511" s="19"/>
+      <c r="E511" s="19" t="s">
+        <v>330</v>
+      </c>
       <c r="F511" s="1" t="s">
         <v>17</v>
       </c>
@@ -23383,7 +23923,9 @@
       <c r="D512" s="7">
         <v>0.64236111111111116</v>
       </c>
-      <c r="E512" s="19"/>
+      <c r="E512" s="19" t="s">
+        <v>377</v>
+      </c>
       <c r="F512" s="1" t="s">
         <v>87</v>
       </c>
@@ -23422,7 +23964,9 @@
       <c r="D513" s="7">
         <v>0.67708333333333337</v>
       </c>
-      <c r="E513" s="19"/>
+      <c r="E513" s="19" t="s">
+        <v>336</v>
+      </c>
       <c r="F513" s="1" t="s">
         <v>289</v>
       </c>
@@ -23461,7 +24005,9 @@
       <c r="D514" s="7">
         <v>0.65625</v>
       </c>
-      <c r="E514" s="19"/>
+      <c r="E514" s="19" t="s">
+        <v>342</v>
+      </c>
       <c r="F514" s="1" t="s">
         <v>15</v>
       </c>
@@ -23500,7 +24046,9 @@
       <c r="D515" s="7">
         <v>0.65902777777777777</v>
       </c>
-      <c r="E515" s="19"/>
+      <c r="E515" s="19" t="s">
+        <v>753</v>
+      </c>
       <c r="F515" s="1" t="s">
         <v>15</v>
       </c>
@@ -23539,7 +24087,9 @@
       <c r="D516" s="7">
         <v>0.62013888888888891</v>
       </c>
-      <c r="E516" s="19"/>
+      <c r="E516" s="19" t="s">
+        <v>450</v>
+      </c>
       <c r="F516" s="1" t="s">
         <v>14</v>
       </c>
@@ -23578,7 +24128,9 @@
       <c r="D517" s="7">
         <v>0.67013888888888884</v>
       </c>
-      <c r="E517" s="19"/>
+      <c r="E517" s="19" t="s">
+        <v>700</v>
+      </c>
       <c r="F517" s="1" t="s">
         <v>14</v>
       </c>
@@ -23617,7 +24169,9 @@
       <c r="D518" s="7">
         <v>0.64652777777777781</v>
       </c>
-      <c r="E518" s="19"/>
+      <c r="E518" s="19" t="s">
+        <v>754</v>
+      </c>
       <c r="F518" s="1" t="s">
         <v>241</v>
       </c>
@@ -23656,7 +24210,9 @@
       <c r="D519" s="7">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E519" s="19"/>
+      <c r="E519" s="19" t="s">
+        <v>421</v>
+      </c>
       <c r="F519" s="1" t="s">
         <v>14</v>
       </c>
@@ -23695,7 +24251,9 @@
       <c r="D520" s="7">
         <v>0.69374999999999998</v>
       </c>
-      <c r="E520" s="19"/>
+      <c r="E520" s="19" t="s">
+        <v>755</v>
+      </c>
       <c r="F520" s="1" t="s">
         <v>17</v>
       </c>
@@ -23734,7 +24292,9 @@
       <c r="D521" s="7">
         <v>0.61250000000000004</v>
       </c>
-      <c r="E521" s="19"/>
+      <c r="E521" s="19" t="s">
+        <v>424</v>
+      </c>
       <c r="F521" s="1" t="s">
         <v>14</v>
       </c>
@@ -23773,7 +24333,9 @@
       <c r="D522" s="7">
         <v>0.63749999999999996</v>
       </c>
-      <c r="E522" s="19"/>
+      <c r="E522" s="19" t="s">
+        <v>751</v>
+      </c>
       <c r="F522" s="1" t="s">
         <v>241</v>
       </c>
@@ -23812,7 +24374,9 @@
       <c r="D523" s="10">
         <v>0.40625</v>
       </c>
-      <c r="E523" s="19"/>
+      <c r="E523" s="19" t="s">
+        <v>345</v>
+      </c>
       <c r="F523" s="1" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
Objective 3 Exploratory Plots_1
</commit_message>
<xml_diff>
--- a/data/raw_data/RAW_WQ Data_TimeModified.xlsx
+++ b/data/raw_data/RAW_WQ Data_TimeModified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17033\Desktop\Modern Applied Data Analysis\William-Norfolk-Project\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9907DD-C97E-40B1-A18B-D1A64FC02060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4052A53C-AEDF-4064-914D-8AED2A46B560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3203" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3203" uniqueCount="755">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1702,9 +1702,6 @@
     <t>03.02.16</t>
   </si>
   <si>
-    <t>03.03.13</t>
-  </si>
-  <si>
     <t>03.03.16</t>
   </si>
   <si>
@@ -1951,9 +1948,6 @@
     <t>07.07.17</t>
   </si>
   <si>
-    <t>07.08.27</t>
-  </si>
-  <si>
     <t>07.11.17</t>
   </si>
   <si>
@@ -2288,6 +2282,9 @@
   </si>
   <si>
     <t>1639</t>
+  </si>
+  <si>
+    <t>07.08.17</t>
   </si>
 </sst>
 </file>
@@ -2719,8 +2716,8 @@
   <dimension ref="A1:O902"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A500" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E524" sqref="E524"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3841,7 +3838,7 @@
     </row>
     <row r="27" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C27" s="6">
         <v>42432</v>
@@ -3883,7 +3880,7 @@
     </row>
     <row r="28" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="22" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C28" s="6">
         <v>42433</v>
@@ -3925,7 +3922,7 @@
     </row>
     <row r="29" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B29" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C29" s="6">
         <v>42434</v>
@@ -3967,7 +3964,7 @@
     </row>
     <row r="30" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C30" s="11">
         <v>42434</v>
@@ -4009,7 +4006,7 @@
     </row>
     <row r="31" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C31" s="6">
         <v>42434</v>
@@ -4051,7 +4048,7 @@
     </row>
     <row r="32" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="22" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C32" s="6">
         <v>42438</v>
@@ -4093,7 +4090,7 @@
     </row>
     <row r="33" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B33" s="22" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C33" s="6">
         <v>42439</v>
@@ -4135,7 +4132,7 @@
     </row>
     <row r="34" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B34" s="22" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C34" s="11">
         <v>42450</v>
@@ -4177,7 +4174,7 @@
     </row>
     <row r="35" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B35" s="22" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C35" s="11">
         <v>42450</v>
@@ -4219,7 +4216,7 @@
     </row>
     <row r="36" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B36" s="22" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C36" s="11">
         <v>42450</v>
@@ -4261,7 +4258,7 @@
     </row>
     <row r="37" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B37" s="22" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C37" s="6">
         <v>42456</v>
@@ -4303,7 +4300,7 @@
     </row>
     <row r="38" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B38" s="22" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C38" s="11">
         <v>42459</v>
@@ -4345,7 +4342,7 @@
     </row>
     <row r="39" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B39" s="22" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C39" s="11">
         <v>42460</v>
@@ -4387,7 +4384,7 @@
     </row>
     <row r="40" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B40" s="22" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C40" s="6">
         <v>42460</v>
@@ -4429,7 +4426,7 @@
     </row>
     <row r="41" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B41" s="22" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C41" s="11">
         <v>42464</v>
@@ -4471,7 +4468,7 @@
     </row>
     <row r="42" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B42" s="22" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C42" s="11">
         <v>42464</v>
@@ -4513,7 +4510,7 @@
     </row>
     <row r="43" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B43" s="22" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C43" s="11">
         <v>42464</v>
@@ -4555,7 +4552,7 @@
     </row>
     <row r="44" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B44" s="22" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C44" s="11">
         <v>42488</v>
@@ -4597,7 +4594,7 @@
     </row>
     <row r="45" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="22" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C45" s="11">
         <v>42488</v>
@@ -4639,7 +4636,7 @@
     </row>
     <row r="46" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B46" s="22" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C46" s="11">
         <v>42497</v>
@@ -4681,7 +4678,7 @@
     </row>
     <row r="47" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B47" s="22" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C47" s="11">
         <v>42498</v>
@@ -4723,7 +4720,7 @@
     </row>
     <row r="48" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="22" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C48" s="11">
         <v>42504</v>
@@ -4765,7 +4762,7 @@
     </row>
     <row r="49" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B49" s="22" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C49" s="11">
         <v>42504</v>
@@ -4807,7 +4804,7 @@
     </row>
     <row r="50" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B50" s="22" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C50" s="11">
         <v>42504</v>
@@ -4849,7 +4846,7 @@
     </row>
     <row r="51" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="22" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C51" s="11">
         <v>42504</v>
@@ -4891,7 +4888,7 @@
     </row>
     <row r="52" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C52" s="11">
         <v>42505</v>
@@ -4933,7 +4930,7 @@
     </row>
     <row r="53" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B53" s="22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C53" s="11">
         <v>42505</v>
@@ -4975,7 +4972,7 @@
     </row>
     <row r="54" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B54" s="22" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C54" s="11">
         <v>42522</v>
@@ -5017,7 +5014,7 @@
     </row>
     <row r="55" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B55" s="22" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C55" s="11">
         <v>42523</v>
@@ -5059,7 +5056,7 @@
     </row>
     <row r="56" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B56" s="22" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C56" s="11">
         <v>42523</v>
@@ -5101,7 +5098,7 @@
     </row>
     <row r="57" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B57" s="22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C57" s="11">
         <v>42524</v>
@@ -5142,7 +5139,7 @@
     </row>
     <row r="58" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B58" s="22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C58" s="11">
         <v>42524</v>
@@ -5184,7 +5181,7 @@
     </row>
     <row r="59" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B59" s="22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C59" s="11">
         <v>42524</v>
@@ -5226,7 +5223,7 @@
     </row>
     <row r="60" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B60" s="22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C60" s="11">
         <v>42524</v>
@@ -5268,7 +5265,7 @@
     </row>
     <row r="61" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B61" s="22" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C61" s="11">
         <v>42525</v>
@@ -5310,7 +5307,7 @@
     </row>
     <row r="62" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B62" s="22" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C62" s="11">
         <v>42525</v>
@@ -5352,7 +5349,7 @@
     </row>
     <row r="63" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B63" s="22" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C63" s="11">
         <v>42526</v>
@@ -5394,7 +5391,7 @@
     </row>
     <row r="64" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B64" s="22" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C64" s="11">
         <v>42529</v>
@@ -5436,7 +5433,7 @@
     </row>
     <row r="65" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B65" s="22" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C65" s="11">
         <v>42538</v>
@@ -5478,7 +5475,7 @@
     </row>
     <row r="66" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B66" s="22" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C66" s="11">
         <v>42538</v>
@@ -5520,7 +5517,7 @@
     </row>
     <row r="67" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B67" s="22" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C67" s="11">
         <v>42539</v>
@@ -5562,7 +5559,7 @@
     </row>
     <row r="68" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B68" s="22" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C68" s="11">
         <v>42539</v>
@@ -5604,7 +5601,7 @@
     </row>
     <row r="69" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B69" s="22" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C69" s="11">
         <v>42540</v>
@@ -5646,7 +5643,7 @@
     </row>
     <row r="70" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B70" s="22" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C70" s="11">
         <v>42540</v>
@@ -5688,7 +5685,7 @@
     </row>
     <row r="71" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B71" s="22" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C71" s="11">
         <v>42540</v>
@@ -5730,7 +5727,7 @@
     </row>
     <row r="72" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B72" s="22" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C72" s="11">
         <v>42541</v>
@@ -5772,7 +5769,7 @@
     </row>
     <row r="73" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B73" s="22" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C73" s="11">
         <v>42543</v>
@@ -5814,7 +5811,7 @@
     </row>
     <row r="74" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B74" s="22" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C74" s="11">
         <v>42543</v>
@@ -5856,7 +5853,7 @@
     </row>
     <row r="75" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B75" s="22" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C75" s="11">
         <v>42544</v>
@@ -5898,7 +5895,7 @@
     </row>
     <row r="76" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B76" s="22" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C76" s="11">
         <v>42544</v>
@@ -5940,7 +5937,7 @@
     </row>
     <row r="77" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77" s="22" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C77" s="11">
         <v>42544</v>
@@ -5982,7 +5979,7 @@
     </row>
     <row r="78" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B78" s="22" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C78" s="11">
         <v>42545</v>
@@ -6024,7 +6021,7 @@
     </row>
     <row r="79" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B79" s="22" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C79" s="11">
         <v>42545</v>
@@ -6066,7 +6063,7 @@
     </row>
     <row r="80" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80" s="22" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C80" s="11">
         <v>42545</v>
@@ -6108,7 +6105,7 @@
     </row>
     <row r="81" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B81" s="22" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C81" s="11">
         <v>42545</v>
@@ -6150,7 +6147,7 @@
     </row>
     <row r="82" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B82" s="22" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C82" s="11">
         <v>42545</v>
@@ -6192,7 +6189,7 @@
     </row>
     <row r="83" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B83" s="22" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C83" s="11">
         <v>42547</v>
@@ -6234,7 +6231,7 @@
     </row>
     <row r="84" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B84" s="22" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C84" s="12">
         <v>42547</v>
@@ -6276,7 +6273,7 @@
     </row>
     <row r="85" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B85" s="22" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C85" s="11">
         <v>42547</v>
@@ -6318,7 +6315,7 @@
     </row>
     <row r="86" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B86" s="22" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C86" s="11">
         <v>42547</v>
@@ -6360,7 +6357,7 @@
     </row>
     <row r="87" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B87" s="22" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C87" s="11">
         <v>42548</v>
@@ -6402,7 +6399,7 @@
     </row>
     <row r="88" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B88" s="22" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C88" s="11">
         <v>42548</v>
@@ -6444,7 +6441,7 @@
     </row>
     <row r="89" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B89" s="22" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C89" s="11">
         <v>42548</v>
@@ -6486,7 +6483,7 @@
     </row>
     <row r="90" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B90" s="22" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C90" s="11">
         <v>42549</v>
@@ -6528,7 +6525,7 @@
     </row>
     <row r="91" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B91" s="22" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C91" s="11">
         <v>42549</v>
@@ -6570,7 +6567,7 @@
     </row>
     <row r="92" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B92" s="22" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C92" s="11">
         <v>42551</v>
@@ -6612,7 +6609,7 @@
     </row>
     <row r="93" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B93" s="22" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C93" s="11">
         <v>42552</v>
@@ -6654,7 +6651,7 @@
     </row>
     <row r="94" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B94" s="22" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C94" s="11">
         <v>42563</v>
@@ -6696,7 +6693,7 @@
     </row>
     <row r="95" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B95" s="22" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C95" s="11">
         <v>42564</v>
@@ -6738,7 +6735,7 @@
     </row>
     <row r="96" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B96" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C96" s="11">
         <v>42565</v>
@@ -6780,7 +6777,7 @@
     </row>
     <row r="97" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B97" s="22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C97" s="11">
         <v>42568</v>
@@ -6822,7 +6819,7 @@
     </row>
     <row r="98" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B98" s="22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C98" s="11">
         <v>42568</v>
@@ -6864,7 +6861,7 @@
     </row>
     <row r="99" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B99" s="22" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C99" s="13">
         <v>42570</v>
@@ -6906,7 +6903,7 @@
     </row>
     <row r="100" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B100" s="22" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C100" s="11">
         <v>42577</v>
@@ -6948,7 +6945,7 @@
     </row>
     <row r="101" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B101" s="22" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C101" s="11">
         <v>42577</v>
@@ -6990,7 +6987,7 @@
     </row>
     <row r="102" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B102" s="22" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C102" s="11">
         <v>42577</v>
@@ -7032,7 +7029,7 @@
     </row>
     <row r="103" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B103" s="22" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C103" s="11">
         <v>42579</v>
@@ -7074,7 +7071,7 @@
     </row>
     <row r="104" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B104" s="22" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C104" s="11">
         <v>42582</v>
@@ -7116,7 +7113,7 @@
     </row>
     <row r="105" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B105" s="22" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C105" s="11">
         <v>42583</v>
@@ -7158,7 +7155,7 @@
     </row>
     <row r="106" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B106" s="22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C106" s="11">
         <v>42594</v>
@@ -7200,7 +7197,7 @@
     </row>
     <row r="107" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B107" s="22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C107" s="11">
         <v>42594</v>
@@ -7242,7 +7239,7 @@
     </row>
     <row r="108" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B108" s="22" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C108" s="11">
         <v>42596</v>
@@ -7284,7 +7281,7 @@
     </row>
     <row r="109" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B109" s="22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C109" s="13">
         <v>42636</v>
@@ -7326,7 +7323,7 @@
     </row>
     <row r="110" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B110" s="22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C110" s="13">
         <v>42636</v>
@@ -7368,7 +7365,7 @@
     </row>
     <row r="111" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B111" s="22" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C111" s="11">
         <v>42667</v>
@@ -7410,7 +7407,7 @@
     </row>
     <row r="112" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B112" s="22" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C112" s="11">
         <v>42667</v>
@@ -7452,7 +7449,7 @@
     </row>
     <row r="113" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B113" s="22" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C113" s="11">
         <v>42667</v>
@@ -7494,7 +7491,7 @@
     </row>
     <row r="114" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B114" s="22" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C114" s="11">
         <v>42668</v>
@@ -7536,7 +7533,7 @@
     </row>
     <row r="115" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B115" s="22" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C115" s="11">
         <v>42668</v>
@@ -7578,7 +7575,7 @@
     </row>
     <row r="116" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B116" s="22" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C116" s="11">
         <v>42669</v>
@@ -7620,7 +7617,7 @@
     </row>
     <row r="117" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B117" s="22" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C117" s="11">
         <v>42695</v>
@@ -7662,7 +7659,7 @@
     </row>
     <row r="118" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B118" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C118" s="11">
         <v>42719</v>
@@ -7704,7 +7701,7 @@
     </row>
     <row r="119" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B119" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C119" s="11">
         <v>42719</v>
@@ -7746,7 +7743,7 @@
     </row>
     <row r="120" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B120" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C120" s="13">
         <v>42719</v>
@@ -7788,7 +7785,7 @@
     </row>
     <row r="121" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B121" s="22" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C121" s="11">
         <v>42746</v>
@@ -7830,7 +7827,7 @@
     </row>
     <row r="122" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="22" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C122" s="11">
         <v>42746</v>
@@ -7872,7 +7869,7 @@
     </row>
     <row r="123" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="22" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C123" s="11">
         <v>42748</v>
@@ -7914,7 +7911,7 @@
     </row>
     <row r="124" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B124" s="22" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C124" s="11">
         <v>42777</v>
@@ -7956,7 +7953,7 @@
     </row>
     <row r="125" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B125" s="22" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C125" s="11">
         <v>42777</v>
@@ -7998,7 +7995,7 @@
     </row>
     <row r="126" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B126" s="22" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C126" s="11">
         <v>42777</v>
@@ -8040,7 +8037,7 @@
     </row>
     <row r="127" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B127" s="22" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C127" s="11">
         <v>42779</v>
@@ -8082,7 +8079,7 @@
     </row>
     <row r="128" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B128" s="22" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C128" s="13">
         <v>42780</v>
@@ -8124,7 +8121,7 @@
     </row>
     <row r="129" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B129" s="22" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C129" s="13">
         <v>42780</v>
@@ -8166,7 +8163,7 @@
     </row>
     <row r="130" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B130" s="22" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C130" s="13">
         <v>42781</v>
@@ -8208,7 +8205,7 @@
     </row>
     <row r="131" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B131" s="22" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C131" s="11">
         <v>42781</v>
@@ -8250,7 +8247,7 @@
     </row>
     <row r="132" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B132" s="22" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C132" s="13">
         <v>42782</v>
@@ -8292,7 +8289,7 @@
     </row>
     <row r="133" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B133" s="22" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C133" s="13">
         <v>42782</v>
@@ -8334,7 +8331,7 @@
     </row>
     <row r="134" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B134" s="22" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C134" s="13">
         <v>42782</v>
@@ -8376,7 +8373,7 @@
     </row>
     <row r="135" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B135" s="22" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C135" s="11">
         <v>42785</v>
@@ -8418,7 +8415,7 @@
     </row>
     <row r="136" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B136" s="22" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C136" s="11">
         <v>42785</v>
@@ -8459,7 +8456,7 @@
     </row>
     <row r="137" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B137" s="22" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C137" s="13">
         <v>42786</v>
@@ -8501,7 +8498,7 @@
     </row>
     <row r="138" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B138" s="22" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C138" s="13">
         <v>42786</v>
@@ -8543,7 +8540,7 @@
     </row>
     <row r="139" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B139" s="22" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C139" s="13">
         <v>42786</v>
@@ -8585,7 +8582,7 @@
     </row>
     <row r="140" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B140" s="22" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C140" s="13">
         <v>42787</v>
@@ -8627,7 +8624,7 @@
     </row>
     <row r="141" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B141" s="22" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C141" s="13">
         <v>42787</v>
@@ -8669,7 +8666,7 @@
     </row>
     <row r="142" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B142" s="22" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C142" s="13">
         <v>42787</v>
@@ -8711,7 +8708,7 @@
     </row>
     <row r="143" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B143" s="22" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C143" s="13">
         <v>42787</v>
@@ -8753,7 +8750,7 @@
     </row>
     <row r="144" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B144" s="22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C144" s="13">
         <v>42792</v>
@@ -8795,7 +8792,7 @@
     </row>
     <row r="145" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B145" s="22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C145" s="13">
         <v>42792</v>
@@ -8837,7 +8834,7 @@
     </row>
     <row r="146" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B146" s="22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C146" s="11">
         <v>42792</v>
@@ -8879,7 +8876,7 @@
     </row>
     <row r="147" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B147" s="22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C147" s="13">
         <v>42792</v>
@@ -8921,7 +8918,7 @@
     </row>
     <row r="148" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B148" s="22" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C148" s="14">
         <v>42793</v>
@@ -8963,7 +8960,7 @@
     </row>
     <row r="149" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B149" s="22" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C149" s="11">
         <v>42793</v>
@@ -9005,7 +9002,7 @@
     </row>
     <row r="150" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B150" s="22" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C150" s="11">
         <v>42793</v>
@@ -9047,7 +9044,7 @@
     </row>
     <row r="151" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B151" s="22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C151" s="13">
         <v>42794</v>
@@ -9089,7 +9086,7 @@
     </row>
     <row r="152" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B152" s="22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C152" s="13">
         <v>42794</v>
@@ -9131,7 +9128,7 @@
     </row>
     <row r="153" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B153" s="22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C153" s="13">
         <v>42794</v>
@@ -9173,7 +9170,7 @@
     </row>
     <row r="154" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B154" s="22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C154" s="13">
         <v>42794</v>
@@ -9215,7 +9212,7 @@
     </row>
     <row r="155" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B155" s="22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C155" s="13">
         <v>42794</v>
@@ -9257,7 +9254,7 @@
     </row>
     <row r="156" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B156" s="22" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C156" s="13">
         <v>42796</v>
@@ -9299,7 +9296,7 @@
     </row>
     <row r="157" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B157" s="22" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C157" s="13">
         <v>42807</v>
@@ -9341,7 +9338,7 @@
     </row>
     <row r="158" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B158" s="22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C158" s="11">
         <v>42812</v>
@@ -9383,7 +9380,7 @@
     </row>
     <row r="159" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B159" s="22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C159" s="11">
         <v>42812</v>
@@ -9425,7 +9422,7 @@
     </row>
     <row r="160" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B160" s="22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C160" s="13">
         <v>42812</v>
@@ -9467,7 +9464,7 @@
     </row>
     <row r="161" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B161" s="22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C161" s="13">
         <v>42812</v>
@@ -9509,7 +9506,7 @@
     </row>
     <row r="162" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B162" s="22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C162" s="13">
         <v>42812</v>
@@ -9551,7 +9548,7 @@
     </row>
     <row r="163" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B163" s="22" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C163" s="13">
         <v>42814</v>
@@ -9593,7 +9590,7 @@
     </row>
     <row r="164" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B164" s="22" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C164" s="13">
         <v>42814</v>
@@ -9635,7 +9632,7 @@
     </row>
     <row r="165" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B165" s="22" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C165" s="13">
         <v>42815</v>
@@ -9677,7 +9674,7 @@
     </row>
     <row r="166" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B166" s="22" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C166" s="11">
         <v>42826</v>
@@ -9719,7 +9716,7 @@
     </row>
     <row r="167" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B167" s="22" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C167" s="14">
         <v>42826</v>
@@ -9761,7 +9758,7 @@
     </row>
     <row r="168" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B168" s="22" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C168" s="11">
         <v>42826</v>
@@ -9803,7 +9800,7 @@
     </row>
     <row r="169" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B169" s="22" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C169" s="13">
         <v>42827</v>
@@ -9845,7 +9842,7 @@
     </row>
     <row r="170" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B170" s="22" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C170" s="13">
         <v>42827</v>
@@ -9887,7 +9884,7 @@
     </row>
     <row r="171" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B171" s="22" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C171" s="13">
         <v>42827</v>
@@ -9929,7 +9926,7 @@
     </row>
     <row r="172" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B172" s="22" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C172" s="13">
         <v>42834</v>
@@ -9971,7 +9968,7 @@
     </row>
     <row r="173" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B173" s="22" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C173" s="13">
         <v>42834</v>
@@ -10013,7 +10010,7 @@
     </row>
     <row r="174" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B174" s="22" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C174" s="13">
         <v>42834</v>
@@ -10055,7 +10052,7 @@
     </row>
     <row r="175" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B175" s="22" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C175" s="13">
         <v>42835</v>
@@ -10097,7 +10094,7 @@
     </row>
     <row r="176" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B176" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C176" s="13">
         <v>42835</v>
@@ -10139,7 +10136,7 @@
     </row>
     <row r="177" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B177" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C177" s="13">
         <v>42835</v>
@@ -10181,7 +10178,7 @@
     </row>
     <row r="178" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B178" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C178" s="13">
         <v>42835</v>
@@ -10223,7 +10220,7 @@
     </row>
     <row r="179" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B179" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C179" s="13">
         <v>42835</v>
@@ -10265,7 +10262,7 @@
     </row>
     <row r="180" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B180" s="22" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C180" s="13">
         <v>42838</v>
@@ -10307,7 +10304,7 @@
     </row>
     <row r="181" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B181" s="22" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C181" s="13">
         <v>42869</v>
@@ -10349,7 +10346,7 @@
     </row>
     <row r="182" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B182" s="22" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C182" s="13">
         <v>42871</v>
@@ -10391,7 +10388,7 @@
     </row>
     <row r="183" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B183" s="22" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C183" s="13">
         <v>42891</v>
@@ -10433,7 +10430,7 @@
     </row>
     <row r="184" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B184" s="22" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C184" s="13">
         <v>42891</v>
@@ -10475,7 +10472,7 @@
     </row>
     <row r="185" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B185" s="22" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C185" s="13">
         <v>42898</v>
@@ -10517,7 +10514,7 @@
     </row>
     <row r="186" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B186" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C186" s="13">
         <v>42898</v>
@@ -10559,7 +10556,7 @@
     </row>
     <row r="187" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B187" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C187" s="13">
         <v>42898</v>
@@ -10601,7 +10598,7 @@
     </row>
     <row r="188" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B188" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C188" s="13">
         <v>42898</v>
@@ -10643,7 +10640,7 @@
     </row>
     <row r="189" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B189" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C189" s="13">
         <v>42898</v>
@@ -10685,7 +10682,7 @@
     </row>
     <row r="190" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B190" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C190" s="13">
         <v>42898</v>
@@ -10727,7 +10724,7 @@
     </row>
     <row r="191" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B191" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C191" s="11">
         <v>42899</v>
@@ -10769,7 +10766,7 @@
     </row>
     <row r="192" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B192" s="22" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C192" s="13">
         <v>42900</v>
@@ -10811,7 +10808,7 @@
     </row>
     <row r="193" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B193" s="22" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C193" s="13">
         <v>42901</v>
@@ -10853,7 +10850,7 @@
     </row>
     <row r="194" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B194" s="22" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C194" s="13">
         <v>42901</v>
@@ -10895,7 +10892,7 @@
     </row>
     <row r="195" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B195" s="22" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C195" s="13">
         <v>42904</v>
@@ -10937,7 +10934,7 @@
     </row>
     <row r="196" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B196" s="22" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C196" s="11">
         <v>42904</v>
@@ -10979,7 +10976,7 @@
     </row>
     <row r="197" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B197" s="22" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C197" s="13">
         <v>42916</v>
@@ -11021,7 +11018,7 @@
     </row>
     <row r="198" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B198" s="22" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C198" s="13">
         <v>42923</v>
@@ -11063,7 +11060,7 @@
     </row>
     <row r="199" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B199" s="22" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C199" s="11">
         <v>42923</v>
@@ -11105,7 +11102,7 @@
     </row>
     <row r="200" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B200" s="22" t="s">
-        <v>643</v>
+        <v>754</v>
       </c>
       <c r="C200" s="13">
         <v>42924</v>
@@ -11147,7 +11144,7 @@
     </row>
     <row r="201" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B201" s="22" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C201" s="11">
         <v>42927</v>
@@ -11189,7 +11186,7 @@
     </row>
     <row r="202" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B202" s="22" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C202" s="13">
         <v>42927</v>
@@ -11231,7 +11228,7 @@
     </row>
     <row r="203" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B203" s="22" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C203" s="13">
         <v>42934</v>
@@ -11273,7 +11270,7 @@
     </row>
     <row r="204" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B204" s="22" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C204" s="11">
         <v>42934</v>
@@ -11315,7 +11312,7 @@
     </row>
     <row r="205" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B205" s="22" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C205" s="13">
         <v>42935</v>
@@ -11357,7 +11354,7 @@
     </row>
     <row r="206" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B206" s="22" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C206" s="13">
         <v>42935</v>
@@ -11399,7 +11396,7 @@
     </row>
     <row r="207" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B207" s="22" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C207" s="13">
         <v>42936</v>
@@ -11441,7 +11438,7 @@
     </row>
     <row r="208" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B208" s="22" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C208" s="13">
         <v>42936</v>
@@ -11483,7 +11480,7 @@
     </row>
     <row r="209" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B209" s="22" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C209" s="13">
         <v>42941</v>
@@ -11525,7 +11522,7 @@
     </row>
     <row r="210" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B210" s="22" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C210" s="11">
         <v>42941</v>
@@ -11567,7 +11564,7 @@
     </row>
     <row r="211" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B211" s="22" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C211" s="11">
         <v>42941</v>
@@ -11609,7 +11606,7 @@
     </row>
     <row r="212" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B212" s="22" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C212" s="13">
         <v>42941</v>
@@ -11651,7 +11648,7 @@
     </row>
     <row r="213" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B213" s="22" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C213" s="13">
         <v>42942</v>
@@ -11693,7 +11690,7 @@
     </row>
     <row r="214" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B214" s="22" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C214" s="13">
         <v>42957</v>
@@ -11735,7 +11732,7 @@
     </row>
     <row r="215" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B215" s="22" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C215" s="13">
         <v>42958</v>
@@ -11777,7 +11774,7 @@
     </row>
     <row r="216" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B216" s="22" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C216" s="13">
         <v>42959</v>
@@ -11819,7 +11816,7 @@
     </row>
     <row r="217" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B217" s="22" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C217" s="13">
         <v>42959</v>
@@ -11861,7 +11858,7 @@
     </row>
     <row r="218" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B218" s="22" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C218" s="13">
         <v>43027</v>
@@ -11902,7 +11899,7 @@
     </row>
     <row r="219" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B219" s="22" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C219" s="11">
         <v>43027</v>
@@ -11943,7 +11940,7 @@
     </row>
     <row r="220" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B220" s="22" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C220" s="13">
         <v>43027</v>
@@ -11984,7 +11981,7 @@
     </row>
     <row r="221" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B221" s="22" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C221" s="13">
         <v>43027</v>
@@ -12025,7 +12022,7 @@
     </row>
     <row r="222" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B222" s="22" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C222" s="13">
         <v>43079</v>
@@ -12066,7 +12063,7 @@
     </row>
     <row r="223" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B223" s="22" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C223" s="11">
         <v>43079</v>
@@ -12107,7 +12104,7 @@
     </row>
     <row r="224" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B224" s="22" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C224" s="13">
         <v>43080</v>
@@ -12148,7 +12145,7 @@
     </row>
     <row r="225" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B225" s="22" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C225" s="13">
         <v>43080</v>
@@ -12189,7 +12186,7 @@
     </row>
     <row r="226" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B226" s="22" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C226" s="13">
         <v>43080</v>
@@ -12230,7 +12227,7 @@
     </row>
     <row r="227" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B227" s="22" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C227" s="13">
         <v>43116</v>
@@ -12271,7 +12268,7 @@
     </row>
     <row r="228" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B228" s="22" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C228" s="13">
         <v>43116</v>
@@ -12312,7 +12309,7 @@
     </row>
     <row r="229" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B229" s="22" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C229" s="13">
         <v>43131</v>
@@ -12353,7 +12350,7 @@
     </row>
     <row r="230" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B230" s="22" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C230" s="13">
         <v>43137</v>
@@ -12394,7 +12391,7 @@
     </row>
     <row r="231" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B231" s="22" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C231" s="11">
         <v>43139</v>
@@ -12435,7 +12432,7 @@
     </row>
     <row r="232" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B232" s="22" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C232" s="11">
         <v>43139</v>
@@ -12476,7 +12473,7 @@
     </row>
     <row r="233" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B233" s="22" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C233" s="13">
         <v>43142</v>
@@ -12517,7 +12514,7 @@
     </row>
     <row r="234" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B234" s="22" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C234" s="13">
         <v>43145</v>
@@ -12558,7 +12555,7 @@
     </row>
     <row r="235" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B235" s="22" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C235" s="14">
         <v>43152</v>
@@ -12599,7 +12596,7 @@
     </row>
     <row r="236" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B236" s="22" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C236" s="13">
         <v>43162</v>
@@ -12640,7 +12637,7 @@
     </row>
     <row r="237" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B237" s="22" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C237" s="14">
         <v>43162</v>
@@ -12681,7 +12678,7 @@
     </row>
     <row r="238" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B238" s="22" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C238" s="13">
         <v>43163</v>
@@ -12722,7 +12719,7 @@
     </row>
     <row r="239" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B239" s="22" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C239" s="11">
         <v>43170</v>
@@ -12763,7 +12760,7 @@
     </row>
     <row r="240" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B240" s="22" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C240" s="14">
         <v>43172</v>
@@ -12804,7 +12801,7 @@
     </row>
     <row r="241" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B241" s="22" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C241" s="13">
         <v>43174</v>
@@ -12845,7 +12842,7 @@
     </row>
     <row r="242" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B242" s="22" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C242" s="11">
         <v>43175</v>
@@ -12886,7 +12883,7 @@
     </row>
     <row r="243" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B243" s="22" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C243" s="13">
         <v>43175</v>
@@ -12927,7 +12924,7 @@
     </row>
     <row r="244" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B244" s="22" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C244" s="13">
         <v>43176</v>
@@ -12968,7 +12965,7 @@
     </row>
     <row r="245" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B245" s="22" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C245" s="11">
         <v>43178</v>
@@ -13009,7 +13006,7 @@
     </row>
     <row r="246" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B246" s="22" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C246" s="13">
         <v>43178</v>
@@ -13050,7 +13047,7 @@
     </row>
     <row r="247" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B247" s="22" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C247" s="13">
         <v>43183</v>
@@ -13091,7 +13088,7 @@
     </row>
     <row r="248" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B248" s="22" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C248" s="13">
         <v>43184</v>
@@ -13132,7 +13129,7 @@
     </row>
     <row r="249" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B249" s="22" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C249" s="13">
         <v>43184</v>
@@ -13173,7 +13170,7 @@
     </row>
     <row r="250" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B250" s="22" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C250" s="13">
         <v>43185</v>
@@ -13214,7 +13211,7 @@
     </row>
     <row r="251" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B251" s="22" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C251" s="13">
         <v>43185</v>
@@ -13255,7 +13252,7 @@
     </row>
     <row r="252" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B252" s="22" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C252" s="13">
         <v>43185</v>
@@ -13296,7 +13293,7 @@
     </row>
     <row r="253" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B253" s="22" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C253" s="13">
         <v>43185</v>
@@ -13337,7 +13334,7 @@
     </row>
     <row r="254" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B254" s="22" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C254" s="11">
         <v>43188</v>
@@ -13378,7 +13375,7 @@
     </row>
     <row r="255" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B255" s="22" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C255" s="13">
         <v>43194</v>
@@ -13419,7 +13416,7 @@
     </row>
     <row r="256" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B256" s="22" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C256" s="13">
         <v>43195</v>
@@ -13460,7 +13457,7 @@
     </row>
     <row r="257" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B257" s="22" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C257" s="13">
         <v>43195</v>
@@ -13501,7 +13498,7 @@
     </row>
     <row r="258" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B258" s="22" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C258" s="11">
         <v>43196</v>
@@ -13542,7 +13539,7 @@
     </row>
     <row r="259" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B259" s="22" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C259" s="13">
         <v>43196</v>
@@ -13583,7 +13580,7 @@
     </row>
     <row r="260" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B260" s="22" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C260" s="13">
         <v>43198</v>
@@ -13624,7 +13621,7 @@
     </row>
     <row r="261" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B261" s="22" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C261" s="13">
         <v>43203</v>
@@ -13665,7 +13662,7 @@
     </row>
     <row r="262" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B262" s="22" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C262" s="13">
         <v>43204</v>
@@ -13706,7 +13703,7 @@
     </row>
     <row r="263" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B263" s="22" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C263" s="13">
         <v>43204</v>
@@ -13747,7 +13744,7 @@
     </row>
     <row r="264" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B264" s="22" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C264" s="13">
         <v>43205</v>
@@ -13788,7 +13785,7 @@
     </row>
     <row r="265" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B265" s="22" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C265" s="13">
         <v>43223</v>
@@ -13829,7 +13826,7 @@
     </row>
     <row r="266" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B266" s="22" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C266" s="14">
         <v>43223</v>
@@ -13870,7 +13867,7 @@
     </row>
     <row r="267" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B267" s="22" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="C267" s="11">
         <v>43224</v>
@@ -13911,7 +13908,7 @@
     </row>
     <row r="268" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B268" s="22" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C268" s="13">
         <v>43232</v>
@@ -13952,7 +13949,7 @@
     </row>
     <row r="269" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B269" s="22" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C269" s="13">
         <v>43233</v>
@@ -13993,7 +13990,7 @@
     </row>
     <row r="270" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B270" s="22" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C270" s="13">
         <v>43252</v>
@@ -14034,7 +14031,7 @@
     </row>
     <row r="271" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B271" s="22" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C271" s="13">
         <v>43252</v>
@@ -14075,7 +14072,7 @@
     </row>
     <row r="272" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B272" s="22" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C272" s="13">
         <v>43253</v>
@@ -14116,7 +14113,7 @@
     </row>
     <row r="273" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B273" s="22" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C273" s="13">
         <v>43255</v>
@@ -14157,7 +14154,7 @@
     </row>
     <row r="274" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B274" s="22" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C274" s="13">
         <v>43255</v>
@@ -14198,7 +14195,7 @@
     </row>
     <row r="275" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B275" s="22" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C275" s="13">
         <v>43256</v>
@@ -14239,7 +14236,7 @@
     </row>
     <row r="276" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B276" s="22" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C276" s="11">
         <v>43258</v>
@@ -14280,7 +14277,7 @@
     </row>
     <row r="277" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B277" s="22" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C277" s="13">
         <v>43260</v>
@@ -14321,7 +14318,7 @@
     </row>
     <row r="278" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B278" s="22" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C278" s="13">
         <v>43263</v>
@@ -14362,7 +14359,7 @@
     </row>
     <row r="279" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B279" s="22" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C279" s="13">
         <v>43263</v>
@@ -14403,7 +14400,7 @@
     </row>
     <row r="280" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B280" s="22" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C280" s="13">
         <v>43264</v>
@@ -14444,7 +14441,7 @@
     </row>
     <row r="281" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B281" s="22" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C281" s="13">
         <v>43265</v>
@@ -14485,7 +14482,7 @@
     </row>
     <row r="282" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B282" s="22" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C282" s="13">
         <v>43266</v>
@@ -14526,7 +14523,7 @@
     </row>
     <row r="283" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B283" s="22" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C283" s="13">
         <v>43269</v>
@@ -14567,7 +14564,7 @@
     </row>
     <row r="284" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B284" s="22" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C284" s="13">
         <v>43270</v>
@@ -14608,7 +14605,7 @@
     </row>
     <row r="285" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B285" s="22" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C285" s="13">
         <v>43279</v>
@@ -14649,7 +14646,7 @@
     </row>
     <row r="286" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B286" s="21" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C286" s="13">
         <v>43279</v>
@@ -14690,7 +14687,7 @@
     </row>
     <row r="287" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B287" s="23" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C287" s="13">
         <v>43279</v>
@@ -14731,7 +14728,7 @@
     </row>
     <row r="288" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B288" s="21" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C288" s="13">
         <v>43279</v>
@@ -14772,7 +14769,7 @@
     </row>
     <row r="289" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B289" s="21" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C289" s="13">
         <v>43279</v>
@@ -14813,7 +14810,7 @@
     </row>
     <row r="290" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B290" s="21" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C290" s="14">
         <v>43279</v>
@@ -14854,7 +14851,7 @@
     </row>
     <row r="291" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B291" s="21" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C291" s="13">
         <v>43279</v>
@@ -14895,7 +14892,7 @@
     </row>
     <row r="292" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B292" s="21" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C292" s="13">
         <v>43280</v>
@@ -14936,7 +14933,7 @@
     </row>
     <row r="293" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B293" s="21" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C293" s="14">
         <v>43279</v>
@@ -14977,7 +14974,7 @@
     </row>
     <row r="294" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B294" s="22" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C294" s="13">
         <v>43280</v>
@@ -15018,7 +15015,7 @@
     </row>
     <row r="295" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B295" s="22" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C295" s="13">
         <v>43280</v>
@@ -15059,7 +15056,7 @@
     </row>
     <row r="296" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B296" s="22" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C296" s="13">
         <v>43280</v>
@@ -15100,7 +15097,7 @@
     </row>
     <row r="297" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B297" s="22" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C297" s="13">
         <v>43280</v>
@@ -15141,7 +15138,7 @@
     </row>
     <row r="298" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B298" s="22" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C298" s="13">
         <v>43280</v>
@@ -16503,7 +16500,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="E331" s="19" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="F331" s="1" t="s">
         <v>10</v>
@@ -16544,7 +16541,7 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="E332" s="19" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="F332" s="1" t="s">
         <v>12</v>
@@ -16626,7 +16623,7 @@
         <v>0.48541666666666666</v>
       </c>
       <c r="E334" s="19" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="F334" s="1" t="s">
         <v>10</v>
@@ -16708,7 +16705,7 @@
         <v>0.49791666666666667</v>
       </c>
       <c r="E336" s="19" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="F336" s="1" t="s">
         <v>10</v>
@@ -16790,7 +16787,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="E338" s="19" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="F338" s="1" t="s">
         <v>10</v>
@@ -16831,7 +16828,7 @@
         <v>0.53611111111111109</v>
       </c>
       <c r="E339" s="19" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="F339" s="1" t="s">
         <v>21</v>
@@ -17241,7 +17238,7 @@
         <v>0.63055555555555554</v>
       </c>
       <c r="E349" s="19" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="F349" s="1" t="s">
         <v>87</v>
@@ -17282,7 +17279,7 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="E350" s="19" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="F350" s="1" t="s">
         <v>22</v>
@@ -17323,7 +17320,7 @@
         <v>0.62708333333333333</v>
       </c>
       <c r="E351" s="19" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="F351" s="1" t="s">
         <v>9</v>
@@ -17364,7 +17361,7 @@
         <v>0.40763888888888888</v>
       </c>
       <c r="E352" s="19" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F352" s="1" t="s">
         <v>15</v>
@@ -17651,7 +17648,7 @@
         <v>0.4201388888888889</v>
       </c>
       <c r="E359" s="19" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F359" s="1" t="s">
         <v>10</v>
@@ -17938,7 +17935,7 @@
         <v>0.60138888888888886</v>
       </c>
       <c r="E366" s="19" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F366" s="1" t="s">
         <v>231</v>
@@ -17979,7 +17976,7 @@
         <v>0.45624999999999999</v>
       </c>
       <c r="E367" s="19" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="F367" s="1" t="s">
         <v>14</v>
@@ -18061,7 +18058,7 @@
         <v>0.40763888888888888</v>
       </c>
       <c r="E369" s="19" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F369" s="1" t="s">
         <v>16</v>
@@ -18102,7 +18099,7 @@
         <v>0.45416666666666666</v>
       </c>
       <c r="E370" s="19" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F370" s="1" t="s">
         <v>22</v>
@@ -18184,7 +18181,7 @@
         <v>0.42152777777777778</v>
       </c>
       <c r="E372" s="19" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="F372" s="1" t="s">
         <v>10</v>
@@ -18389,7 +18386,7 @@
         <v>0.63958333333333328</v>
       </c>
       <c r="E377" s="19" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="F377" s="1" t="s">
         <v>16</v>
@@ -18553,7 +18550,7 @@
         <v>0.43611111111111112</v>
       </c>
       <c r="E381" s="19" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="F381" s="1" t="s">
         <v>10</v>
@@ -18594,7 +18591,7 @@
         <v>0.61111111111111116</v>
       </c>
       <c r="E382" s="19" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="F382" s="1" t="s">
         <v>197</v>
@@ -18758,7 +18755,7 @@
         <v>0.65486111111111112</v>
       </c>
       <c r="E386" s="19" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="F386" s="1" t="s">
         <v>197</v>
@@ -18922,7 +18919,7 @@
         <v>0.63958333333333328</v>
       </c>
       <c r="E390" s="19" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="F390" s="1" t="s">
         <v>11</v>
@@ -18963,7 +18960,7 @@
         <v>0.68541666666666667</v>
       </c>
       <c r="E391" s="19" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="F391" s="1" t="s">
         <v>7</v>
@@ -19127,7 +19124,7 @@
         <v>0.46041666666666664</v>
       </c>
       <c r="E395" s="19" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="F395" s="1" t="s">
         <v>245</v>
@@ -19168,7 +19165,7 @@
         <v>0.61597222222222225</v>
       </c>
       <c r="E396" s="19" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F396" s="1" t="s">
         <v>22</v>
@@ -19209,7 +19206,7 @@
         <v>0.61944444444444446</v>
       </c>
       <c r="E397" s="19" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F397" s="1" t="s">
         <v>22</v>
@@ -19455,7 +19452,7 @@
         <v>0.47083333333333333</v>
       </c>
       <c r="E403" s="19" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="F403" s="1" t="s">
         <v>87</v>
@@ -19496,7 +19493,7 @@
         <v>0.61041666666666672</v>
       </c>
       <c r="E404" s="19" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F404" s="1" t="s">
         <v>10</v>
@@ -19947,7 +19944,7 @@
         <v>0.61597222222222225</v>
       </c>
       <c r="E415" s="19" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F415" s="1" t="s">
         <v>10</v>
@@ -20111,7 +20108,7 @@
         <v>0.68888888888888888</v>
       </c>
       <c r="E419" s="19" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="F419" s="1" t="s">
         <v>7</v>
@@ -20152,7 +20149,7 @@
         <v>0.69097222222222221</v>
       </c>
       <c r="E420" s="19" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="F420" s="1" t="s">
         <v>21</v>
@@ -20234,7 +20231,7 @@
         <v>0.4201388888888889</v>
       </c>
       <c r="E422" s="19" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F422" s="1" t="s">
         <v>10</v>
@@ -20316,7 +20313,7 @@
         <v>0.58958333333333335</v>
       </c>
       <c r="E424" s="19" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F424" s="1" t="s">
         <v>12</v>
@@ -20357,7 +20354,7 @@
         <v>0.61111111111111116</v>
       </c>
       <c r="E425" s="19" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="F425" s="1" t="s">
         <v>107</v>
@@ -20439,7 +20436,7 @@
         <v>0.61319444444444449</v>
       </c>
       <c r="E427" s="19" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F427" s="1" t="s">
         <v>15</v>
@@ -20685,7 +20682,7 @@
         <v>0.65833333333333333</v>
       </c>
       <c r="E433" s="19" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F433" s="1" t="s">
         <v>261</v>
@@ -20726,7 +20723,7 @@
         <v>0.4201388888888889</v>
       </c>
       <c r="E434" s="19" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F434" s="1" t="s">
         <v>120</v>
@@ -20808,7 +20805,7 @@
         <v>0.52430555555555558</v>
       </c>
       <c r="E436" s="19" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F436" s="1" t="s">
         <v>11</v>
@@ -20849,7 +20846,7 @@
         <v>0.55486111111111114</v>
       </c>
       <c r="E437" s="19" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F437" s="1" t="s">
         <v>12</v>
@@ -20890,7 +20887,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="E438" s="19" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F438" s="1" t="s">
         <v>12</v>
@@ -21013,7 +21010,7 @@
         <v>0.61388888888888893</v>
       </c>
       <c r="E441" s="19" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F441" s="1" t="s">
         <v>268</v>
@@ -21218,7 +21215,7 @@
         <v>0.6020833333333333</v>
       </c>
       <c r="E446" s="19" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F446" s="1" t="s">
         <v>11</v>
@@ -21382,7 +21379,7 @@
         <v>0.40486111111111112</v>
       </c>
       <c r="E450" s="19" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F450" s="1" t="s">
         <v>10</v>
@@ -21464,7 +21461,7 @@
         <v>0.68194444444444446</v>
       </c>
       <c r="E452" s="19" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F452" s="1" t="s">
         <v>21</v>
@@ -21587,7 +21584,7 @@
         <v>0.44861111111111113</v>
       </c>
       <c r="E455" s="19" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F455" s="1" t="s">
         <v>120</v>
@@ -21669,7 +21666,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E457" s="19" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F457" s="1" t="s">
         <v>14</v>
@@ -21710,7 +21707,7 @@
         <v>0.66597222222222219</v>
       </c>
       <c r="E458" s="19" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F458" s="1" t="s">
         <v>14</v>
@@ -21792,7 +21789,7 @@
         <v>0.45763888888888887</v>
       </c>
       <c r="E460" s="19" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="F460" s="1" t="s">
         <v>14</v>
@@ -21833,7 +21830,7 @@
         <v>0.65208333333333335</v>
       </c>
       <c r="E461" s="19" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F461" s="1" t="s">
         <v>87</v>
@@ -21915,7 +21912,7 @@
         <v>0.42291666666666666</v>
       </c>
       <c r="E463" s="19" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F463" s="1" t="s">
         <v>9</v>
@@ -21956,7 +21953,7 @@
         <v>0.40694444444444444</v>
       </c>
       <c r="E464" s="19" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="F464" s="1" t="s">
         <v>17</v>
@@ -22038,7 +22035,7 @@
         <v>0.42291666666666666</v>
       </c>
       <c r="E466" s="19" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F466" s="1" t="s">
         <v>9</v>
@@ -22202,7 +22199,7 @@
         <v>0.60833333333333328</v>
       </c>
       <c r="E470" s="19" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F470" s="1" t="s">
         <v>13</v>
@@ -22284,7 +22281,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="E472" s="19" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F472" s="1" t="s">
         <v>19</v>
@@ -22448,7 +22445,7 @@
         <v>0.63680555555555551</v>
       </c>
       <c r="E476" s="19" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F476" s="1" t="s">
         <v>87</v>
@@ -22530,7 +22527,7 @@
         <v>0.4</v>
       </c>
       <c r="E478" s="19" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F478" s="1" t="s">
         <v>280</v>
@@ -22694,7 +22691,7 @@
         <v>0.44166666666666665</v>
       </c>
       <c r="E482" s="19" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="F482" s="1" t="s">
         <v>17</v>
@@ -22776,7 +22773,7 @@
         <v>0.68194444444444446</v>
       </c>
       <c r="E484" s="19" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F484" s="1" t="s">
         <v>18</v>
@@ -22940,7 +22937,7 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="E488" s="19" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="F488" s="1" t="s">
         <v>284</v>
@@ -22981,7 +22978,7 @@
         <v>0.48333333333333334</v>
       </c>
       <c r="E489" s="19" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="F489" s="1" t="s">
         <v>120</v>
@@ -23104,7 +23101,7 @@
         <v>0.42777777777777776</v>
       </c>
       <c r="E492" s="19" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="F492" s="1" t="s">
         <v>15</v>
@@ -23391,7 +23388,7 @@
         <v>0.41388888888888886</v>
       </c>
       <c r="E499" s="19" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="F499" s="1" t="s">
         <v>14</v>
@@ -23473,7 +23470,7 @@
         <v>0.65138888888888891</v>
       </c>
       <c r="E501" s="19" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F501" s="1" t="s">
         <v>87</v>
@@ -23514,7 +23511,7 @@
         <v>0.69722222222222219</v>
       </c>
       <c r="E502" s="19" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F502" s="1" t="s">
         <v>11</v>
@@ -24047,7 +24044,7 @@
         <v>0.65902777777777777</v>
       </c>
       <c r="E515" s="19" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F515" s="1" t="s">
         <v>15</v>
@@ -24129,7 +24126,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="E517" s="19" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="F517" s="1" t="s">
         <v>14</v>
@@ -24170,7 +24167,7 @@
         <v>0.64652777777777781</v>
       </c>
       <c r="E518" s="19" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="F518" s="1" t="s">
         <v>241</v>
@@ -24252,7 +24249,7 @@
         <v>0.69374999999999998</v>
       </c>
       <c r="E520" s="19" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F520" s="1" t="s">
         <v>17</v>
@@ -24334,7 +24331,7 @@
         <v>0.63749999999999996</v>
       </c>
       <c r="E522" s="19" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="F522" s="1" t="s">
         <v>241</v>

</xml_diff>